<commit_message>
Update changelog for 2.5 alpha
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jack\Dropbox\Scratch\OpenSolverNew\OpenSolver2.4\OpenSolver Release\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="13905"/>
   </bookViews>
@@ -20,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$83</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$90</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -563,6 +568,24 @@
       </rPr>
       <t>≤,5≥.</t>
     </r>
+  </si>
+  <si>
+    <t>Version 2.5 alpha</t>
+  </si>
+  <si>
+    <t>Support for using the Gurobi LP/IP solver if a user has this installed on their machine</t>
+  </si>
+  <si>
+    <t>Support for solving non-linear models using both NOMAD and the cloud-based NEOS servers</t>
+  </si>
+  <si>
+    <t>Reporting of dual variables and sensitivity analysis</t>
+  </si>
+  <si>
+    <t>Many small bux fixes and feature enhancements</t>
+  </si>
+  <si>
+    <t>Updated CBC.exe to version 2.8.8</t>
   </si>
 </sst>
 </file>
@@ -647,6 +670,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -694,7 +720,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -729,7 +755,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -939,10 +965,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T195"/>
+  <dimension ref="A1:T202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,498 +1035,509 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C10" s="1">
-        <v>41324</v>
+        <v>41809</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="C11" s="1"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>170</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>171</v>
+      </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>172</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>173</v>
+      </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="A16" s="2"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="1"/>
+      <c r="A17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="1">
+        <v>41324</v>
+      </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C18" s="1"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C19" s="1"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C20" s="1"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21" s="1"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C22" s="1"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C23" s="1"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C24" s="1"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C25" s="1"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C26" s="1"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C27" s="1"/>
       <c r="H27" s="5"/>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="H28" s="5"/>
+    </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="1">
-        <v>41211</v>
-      </c>
+      <c r="A29" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>150</v>
-      </c>
+      <c r="A30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="1">
+        <v>41211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C40" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C44" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C49" s="1">
         <v>40963</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="1">
-        <v>40882</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="1"/>
+        <v>137</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="1"/>
+      <c r="A51" s="4" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="1"/>
+        <v>139</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+      <c r="A53" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54" s="1">
-        <v>40877</v>
-      </c>
+      <c r="A54" s="2"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55" s="1"/>
+      <c r="A55" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="1">
+        <v>40882</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>131</v>
+      <c r="A56" t="s">
+        <v>133</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>130</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
+      <c r="A58" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" s="1">
-        <v>40858</v>
-      </c>
+      <c r="A59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="1"/>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>122</v>
+      <c r="A61" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="1">
+        <v>40877</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>123</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>125</v>
-      </c>
+      <c r="A63" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>126</v>
-      </c>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+      <c r="A66" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="1">
+        <v>40858</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C67" s="1">
-        <v>40815</v>
-      </c>
+      <c r="A67" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>102</v>
+      <c r="A68" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>113</v>
-      </c>
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>114</v>
+      <c r="A74" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="1">
+        <v>40815</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>115</v>
+      <c r="A75" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
+      <c r="A81" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C82" s="1">
-        <v>40764</v>
+      <c r="A82" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B85" s="5"/>
+        <v>118</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
+      <c r="A87" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C88" s="1">
-        <v>40755</v>
-      </c>
+      <c r="A88" s="2"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>65</v>
+      <c r="A89" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="1">
+        <v>40764</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="5" t="s">
-        <v>64</v>
+      <c r="A91" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>67</v>
-      </c>
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
+      <c r="A93" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>68</v>
-      </c>
+      <c r="A94" s="4"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>69</v>
+      <c r="A95" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="1">
+        <v>40755</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>72</v>
+      <c r="B98" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>73</v>
+      <c r="B99" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,512 +1545,545 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>76</v>
+      <c r="A103" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
+      <c r="A104" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>79</v>
-      </c>
+      <c r="A107" s="4"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>80</v>
+      <c r="A108" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>81</v>
+      <c r="A109" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="4"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="4"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="4"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C129" s="1">
         <v>40731</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>60</v>
       </c>
-      <c r="C123" s="1"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
+      <c r="C130" s="1"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C124" s="1"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C125" s="1"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C126" s="1"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
+      <c r="C133" s="1"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C135" s="1">
         <v>40610</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C138" s="1">
         <v>40606</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>13</v>
+      <c r="B146" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>19</v>
+      <c r="B151" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
-        <v>20</v>
+      <c r="A153" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
-        <v>37</v>
+      <c r="A156" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>25</v>
+      <c r="B162" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>54</v>
+      <c r="B167" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>51</v>
+      <c r="B171" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>52</v>
+      <c r="A172" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B174" t="s">
-        <v>39</v>
+      <c r="A174" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>33</v>
+      <c r="A176" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B181" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C180" s="3">
-        <v>40407</v>
-      </c>
-    </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C184" s="3">
-        <v>40375</v>
-      </c>
-    </row>
-    <row r="185" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B185" s="7"/>
-      <c r="C185" s="7"/>
-      <c r="D185" s="7"/>
-      <c r="E185" s="7"/>
-      <c r="F185" s="7"/>
-      <c r="G185" s="7"/>
-      <c r="H185" s="7"/>
-      <c r="I185" s="7"/>
-      <c r="J185" s="7"/>
-      <c r="K185" s="7"/>
-      <c r="L185" s="7"/>
-      <c r="M185" s="7"/>
-      <c r="N185" s="7"/>
-      <c r="O185" s="7"/>
-      <c r="P185" s="7"/>
-      <c r="Q185" s="7"/>
-      <c r="R185" s="7"/>
-      <c r="S185" s="7"/>
-      <c r="T185" s="7"/>
     </row>
     <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C187" s="3">
+        <v>40407</v>
+      </c>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C191" s="3">
+        <v>40375</v>
+      </c>
+    </row>
+    <row r="192" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7"/>
+      <c r="E192" s="7"/>
+      <c r="F192" s="7"/>
+      <c r="G192" s="7"/>
+      <c r="H192" s="7"/>
+      <c r="I192" s="7"/>
+      <c r="J192" s="7"/>
+      <c r="K192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="7"/>
+      <c r="N192" s="7"/>
+      <c r="O192" s="7"/>
+      <c r="P192" s="7"/>
+      <c r="Q192" s="7"/>
+      <c r="R192" s="7"/>
+      <c r="S192" s="7"/>
+      <c r="T192" s="7"/>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C187" s="3">
+      <c r="C194" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="6" t="s">
+    <row r="195" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B188" s="6"/>
-      <c r="C188" s="6"/>
-      <c r="D188" s="6"/>
-      <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
-      <c r="G188" s="6"/>
-      <c r="H188" s="6"/>
-      <c r="I188" s="6"/>
-      <c r="J188" s="6"/>
-      <c r="K188" s="6"/>
-      <c r="L188" s="6"/>
-      <c r="M188" s="6"/>
-      <c r="N188" s="6"/>
-      <c r="O188" s="6"/>
-      <c r="P188" s="6"/>
-      <c r="Q188" s="6"/>
-      <c r="R188" s="6"/>
-      <c r="S188" s="6"/>
-      <c r="T188" s="6"/>
-    </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A190" s="2" t="s">
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
+      <c r="E195" s="6"/>
+      <c r="F195" s="6"/>
+      <c r="G195" s="6"/>
+      <c r="H195" s="6"/>
+      <c r="I195" s="6"/>
+      <c r="J195" s="6"/>
+      <c r="K195" s="6"/>
+      <c r="L195" s="6"/>
+      <c r="M195" s="6"/>
+      <c r="N195" s="6"/>
+      <c r="O195" s="6"/>
+      <c r="P195" s="6"/>
+      <c r="Q195" s="6"/>
+      <c r="R195" s="6"/>
+      <c r="S195" s="6"/>
+      <c r="T195" s="6"/>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C190" s="3">
+      <c r="C197" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="6" t="s">
+    <row r="198" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B191" s="6"/>
-      <c r="C191" s="6"/>
-      <c r="D191" s="6"/>
-      <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
-      <c r="G191" s="6"/>
-      <c r="H191" s="6"/>
-      <c r="I191" s="6"/>
-      <c r="J191" s="6"/>
-      <c r="K191" s="6"/>
-      <c r="L191" s="6"/>
-      <c r="M191" s="6"/>
-      <c r="N191" s="6"/>
-      <c r="O191" s="6"/>
-      <c r="P191" s="6"/>
-      <c r="Q191" s="6"/>
-      <c r="R191" s="6"/>
-      <c r="S191" s="6"/>
-      <c r="T191" s="6"/>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+      <c r="J198" s="6"/>
+      <c r="K198" s="6"/>
+      <c r="L198" s="6"/>
+      <c r="M198" s="6"/>
+      <c r="N198" s="6"/>
+      <c r="O198" s="6"/>
+      <c r="P198" s="6"/>
+      <c r="Q198" s="6"/>
+      <c r="R198" s="6"/>
+      <c r="S198" s="6"/>
+      <c r="T198" s="6"/>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C194" s="3">
+      <c r="C201" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A185:T185"/>
-    <mergeCell ref="A188:T188"/>
-    <mergeCell ref="A191:T191"/>
+    <mergeCell ref="A192:T192"/>
+    <mergeCell ref="A195:T195"/>
+    <mergeCell ref="A198:T198"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B91" r:id="rId1"/>
+    <hyperlink ref="B98" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Changelog to mention no-negativity issues
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$90</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$91</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -34,12 +34,12 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -576,9 +576,6 @@
     <t>Support for using the Gurobi LP/IP solver if a user has this installed on their machine</t>
   </si>
   <si>
-    <t>Support for solving non-linear models using both NOMAD and the cloud-based NEOS servers</t>
-  </si>
-  <si>
     <t>Reporting of dual variables and sensitivity analysis</t>
   </si>
   <si>
@@ -586,6 +583,12 @@
   </si>
   <si>
     <t>Updated CBC.exe to version 2.8.8</t>
+  </si>
+  <si>
+    <t>Support for cloud-based NEOS server for CBC solver</t>
+  </si>
+  <si>
+    <t>Support for solving non-linear models using both NOMAD and the cloud-based NEOS servers (assuming non-negativity currently doesn't work correctly for non-linear NEOS, all variables are assumed positive, not just unconstrained ones)</t>
   </si>
 </sst>
 </file>
@@ -965,10 +968,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T202"/>
+  <dimension ref="A1:T203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1047,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" s="1"/>
       <c r="H11" s="5"/>
@@ -1057,1033 +1060,1039 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="2"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>41324</v>
       </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="1"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C19" s="1"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" s="1"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C21" s="1"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C22" s="1"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C23" s="1"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C24" s="1"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C25" s="1"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C26" s="1"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C27" s="1"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C28" s="1"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" s="1"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C30" s="1"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C31" s="1"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C32" s="1"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C33" s="1"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" s="1"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C37" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-    </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C41" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-    </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C45" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-    </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C50" s="1">
         <v>40963</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-    </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C56" s="1">
         <v>40882</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>133</v>
-      </c>
-      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C62" s="1">
         <v>40877</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-    </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C67" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>122</v>
-      </c>
+      <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-    </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C75" s="1">
         <v>40815</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-    </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C90" s="1">
         <v>40764</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>96</v>
-      </c>
-      <c r="B92" s="5"/>
+        <v>94</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="5"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C96" s="1">
         <v>40755</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-    </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>68</v>
-      </c>
+      <c r="A101" s="4"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-    </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>74</v>
-      </c>
+      <c r="A108" s="4"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-    </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>77</v>
-      </c>
+      <c r="A112" s="4"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-    </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>85</v>
-      </c>
+      <c r="A121" s="4"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
-    </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>88</v>
-      </c>
+      <c r="A125" s="4"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2"/>
-    </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C130" s="1">
         <v>40731</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>60</v>
-      </c>
-      <c r="C130" s="1"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C131" s="1"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C133" s="1"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+      <c r="C134" s="1"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C136" s="1">
         <v>40610</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C139" s="1">
         <v>40606</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B182" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C187" s="3">
+      <c r="C188" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C191" s="3">
+      <c r="C192" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="6" t="s">
+    <row r="193" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B192" s="7"/>
-      <c r="C192" s="7"/>
-      <c r="D192" s="7"/>
-      <c r="E192" s="7"/>
-      <c r="F192" s="7"/>
-      <c r="G192" s="7"/>
-      <c r="H192" s="7"/>
-      <c r="I192" s="7"/>
-      <c r="J192" s="7"/>
-      <c r="K192" s="7"/>
-      <c r="L192" s="7"/>
-      <c r="M192" s="7"/>
-      <c r="N192" s="7"/>
-      <c r="O192" s="7"/>
-      <c r="P192" s="7"/>
-      <c r="Q192" s="7"/>
-      <c r="R192" s="7"/>
-      <c r="S192" s="7"/>
-      <c r="T192" s="7"/>
-    </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
+      <c r="B193" s="7"/>
+      <c r="C193" s="7"/>
+      <c r="D193" s="7"/>
+      <c r="E193" s="7"/>
+      <c r="F193" s="7"/>
+      <c r="G193" s="7"/>
+      <c r="H193" s="7"/>
+      <c r="I193" s="7"/>
+      <c r="J193" s="7"/>
+      <c r="K193" s="7"/>
+      <c r="L193" s="7"/>
+      <c r="M193" s="7"/>
+      <c r="N193" s="7"/>
+      <c r="O193" s="7"/>
+      <c r="P193" s="7"/>
+      <c r="Q193" s="7"/>
+      <c r="R193" s="7"/>
+      <c r="S193" s="7"/>
+      <c r="T193" s="7"/>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C194" s="3">
+      <c r="C195" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="6" t="s">
+    <row r="196" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B195" s="6"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
-      <c r="G195" s="6"/>
-      <c r="H195" s="6"/>
-      <c r="I195" s="6"/>
-      <c r="J195" s="6"/>
-      <c r="K195" s="6"/>
-      <c r="L195" s="6"/>
-      <c r="M195" s="6"/>
-      <c r="N195" s="6"/>
-      <c r="O195" s="6"/>
-      <c r="P195" s="6"/>
-      <c r="Q195" s="6"/>
-      <c r="R195" s="6"/>
-      <c r="S195" s="6"/>
-      <c r="T195" s="6"/>
-    </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+      <c r="E196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
+      <c r="H196" s="6"/>
+      <c r="I196" s="6"/>
+      <c r="J196" s="6"/>
+      <c r="K196" s="6"/>
+      <c r="L196" s="6"/>
+      <c r="M196" s="6"/>
+      <c r="N196" s="6"/>
+      <c r="O196" s="6"/>
+      <c r="P196" s="6"/>
+      <c r="Q196" s="6"/>
+      <c r="R196" s="6"/>
+      <c r="S196" s="6"/>
+      <c r="T196" s="6"/>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C197" s="3">
+      <c r="C198" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="6" t="s">
+    <row r="199" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B198" s="6"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="6"/>
-      <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
-      <c r="G198" s="6"/>
-      <c r="H198" s="6"/>
-      <c r="I198" s="6"/>
-      <c r="J198" s="6"/>
-      <c r="K198" s="6"/>
-      <c r="L198" s="6"/>
-      <c r="M198" s="6"/>
-      <c r="N198" s="6"/>
-      <c r="O198" s="6"/>
-      <c r="P198" s="6"/>
-      <c r="Q198" s="6"/>
-      <c r="R198" s="6"/>
-      <c r="S198" s="6"/>
-      <c r="T198" s="6"/>
-    </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
+      <c r="D199" s="6"/>
+      <c r="E199" s="6"/>
+      <c r="F199" s="6"/>
+      <c r="G199" s="6"/>
+      <c r="H199" s="6"/>
+      <c r="I199" s="6"/>
+      <c r="J199" s="6"/>
+      <c r="K199" s="6"/>
+      <c r="L199" s="6"/>
+      <c r="M199" s="6"/>
+      <c r="N199" s="6"/>
+      <c r="O199" s="6"/>
+      <c r="P199" s="6"/>
+      <c r="Q199" s="6"/>
+      <c r="R199" s="6"/>
+      <c r="S199" s="6"/>
+      <c r="T199" s="6"/>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C201" s="3">
+      <c r="C202" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A192:T192"/>
-    <mergeCell ref="A195:T195"/>
-    <mergeCell ref="A198:T198"/>
+    <mergeCell ref="A193:T193"/>
+    <mergeCell ref="A196:T196"/>
+    <mergeCell ref="A199:T199"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B98" r:id="rId1"/>
+    <hyperlink ref="B99" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change release date to 20/06/2014
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$91</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$90</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="174">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -372,12 +372,6 @@
   </si>
   <si>
     <t>Added "Show optimisation progress while solving"  (being Solver's "Show Iteration Results") to the OpenSolver options dialog</t>
-  </si>
-  <si>
-    <t>3/</t>
-  </si>
-  <si>
-    <t>Allow OpenSolver to handle models with no objective (which Solver can handle)</t>
   </si>
   <si>
     <t>Improved operation of Options dialog, including proper sycnronisation of values when opened from the Model dialog</t>
@@ -968,10 +962,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T203"/>
+  <dimension ref="A1:T202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,370 +1018,366 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41810</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C10" s="1">
-        <v>41809</v>
-      </c>
+      <c r="A10" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="1"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>168</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>172</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="1">
+        <v>41324</v>
+      </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="1">
-        <v>41324</v>
-      </c>
+      <c r="A18" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C19" s="1"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" s="1"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C21" s="1"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C22" s="1"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C23" s="1"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C24" s="1"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C25" s="1"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" s="1"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C27" s="1"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C28" s="1"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" s="1"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C30" s="1"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C31" s="1"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C32" s="1"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C33" s="1"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="1"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="H35" s="5"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="1">
+        <v>41211</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>148</v>
       </c>
-      <c r="C37" s="1">
-        <v>41211</v>
-      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>150</v>
+      <c r="A38" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="A39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="1">
+        <v>41176</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="1">
-        <v>41176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>147</v>
-      </c>
+      <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="1">
+        <v>41157</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="1">
-        <v>41157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>143</v>
-      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="1">
+        <v>40963</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C50" s="1">
-        <v>40963</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>140</v>
-      </c>
+      <c r="A54" s="2"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
+      <c r="A55" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="1">
+        <v>40882</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C56" s="1">
-        <v>40882</v>
-      </c>
+      <c r="A56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="1"/>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
+      <c r="A61" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="1">
+        <v>40877</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="1">
-        <v>40877</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>130</v>
-      </c>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+      <c r="A66" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" s="1">
+        <v>40858</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C67" s="1">
-        <v>40858</v>
-      </c>
+      <c r="A67" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C68" s="1"/>
+      <c r="A68" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1397,7 +1387,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1406,69 +1396,69 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>126</v>
-      </c>
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="1">
+        <v>40815</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C75" s="1">
-        <v>40815</v>
+      <c r="A75" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>102</v>
+      <c r="A76" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1478,621 +1468,616 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>119</v>
-      </c>
+      <c r="A88" s="2"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
+      <c r="A89" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="1">
+        <v>40764</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C90" s="1">
-        <v>40764</v>
+      <c r="A90" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>94</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>96</v>
-      </c>
-      <c r="B93" s="5"/>
+        <v>95</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>95</v>
-      </c>
+      <c r="A94" s="4"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
+      <c r="A95" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="1">
+        <v>40755</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C96" s="1">
-        <v>40755</v>
+      <c r="A96" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>66</v>
+      <c r="B98" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="5" t="s">
-        <v>64</v>
+      <c r="B99" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>67</v>
-      </c>
+      <c r="A100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
+      <c r="A101" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>73</v>
-      </c>
+      <c r="A107" s="4"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
+      <c r="A108" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>75</v>
+      <c r="B110" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>76</v>
-      </c>
+      <c r="A111" s="4"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
+      <c r="A112" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>78</v>
+      <c r="B114" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>84</v>
-      </c>
+      <c r="A120" s="4"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
+      <c r="A121" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>87</v>
-      </c>
+      <c r="A124" s="4"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
+      <c r="A125" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>90</v>
-      </c>
+      <c r="A128" s="2"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="2"/>
+      <c r="A129" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C129" s="1">
+        <v>40731</v>
+      </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C130" s="1">
-        <v>40731</v>
-      </c>
+      <c r="A130" t="s">
+        <v>60</v>
+      </c>
+      <c r="C130" s="1"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>60</v>
+      <c r="A131" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C131" s="1"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C134" s="1"/>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C135" s="1">
+        <v>40610</v>
+      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C136" s="1">
-        <v>40610</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A136" t="s">
         <v>58</v>
       </c>
     </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" s="1">
+        <v>40606</v>
+      </c>
+    </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C139" s="1">
-        <v>40606</v>
+      <c r="A139" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>4</v>
+      <c r="B143" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
-        <v>53</v>
+      <c r="A149" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>10</v>
+      <c r="B150" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
-        <v>24</v>
+      <c r="A153" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>13</v>
+      <c r="B154" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
-        <v>15</v>
+      <c r="A156" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>16</v>
+      <c r="B157" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>17</v>
+      <c r="A158" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>19</v>
+      <c r="B159" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>38</v>
+      <c r="A165" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>22</v>
+      <c r="B166" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
-        <v>31</v>
+      <c r="A169" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>25</v>
+      <c r="B170" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>32</v>
+      <c r="A172" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>27</v>
+      <c r="B173" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>28</v>
+      <c r="A174" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>54</v>
+      <c r="B175" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="A176" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B181" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C188" s="3">
+      <c r="C187" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C192" s="3">
+      <c r="C191" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="6" t="s">
+    <row r="192" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B193" s="7"/>
-      <c r="C193" s="7"/>
-      <c r="D193" s="7"/>
-      <c r="E193" s="7"/>
-      <c r="F193" s="7"/>
-      <c r="G193" s="7"/>
-      <c r="H193" s="7"/>
-      <c r="I193" s="7"/>
-      <c r="J193" s="7"/>
-      <c r="K193" s="7"/>
-      <c r="L193" s="7"/>
-      <c r="M193" s="7"/>
-      <c r="N193" s="7"/>
-      <c r="O193" s="7"/>
-      <c r="P193" s="7"/>
-      <c r="Q193" s="7"/>
-      <c r="R193" s="7"/>
-      <c r="S193" s="7"/>
-      <c r="T193" s="7"/>
-    </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A195" s="2" t="s">
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7"/>
+      <c r="E192" s="7"/>
+      <c r="F192" s="7"/>
+      <c r="G192" s="7"/>
+      <c r="H192" s="7"/>
+      <c r="I192" s="7"/>
+      <c r="J192" s="7"/>
+      <c r="K192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="7"/>
+      <c r="N192" s="7"/>
+      <c r="O192" s="7"/>
+      <c r="P192" s="7"/>
+      <c r="Q192" s="7"/>
+      <c r="R192" s="7"/>
+      <c r="S192" s="7"/>
+      <c r="T192" s="7"/>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C195" s="3">
+      <c r="C194" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="6" t="s">
+    <row r="195" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B196" s="6"/>
-      <c r="C196" s="6"/>
-      <c r="D196" s="6"/>
-      <c r="E196" s="6"/>
-      <c r="F196" s="6"/>
-      <c r="G196" s="6"/>
-      <c r="H196" s="6"/>
-      <c r="I196" s="6"/>
-      <c r="J196" s="6"/>
-      <c r="K196" s="6"/>
-      <c r="L196" s="6"/>
-      <c r="M196" s="6"/>
-      <c r="N196" s="6"/>
-      <c r="O196" s="6"/>
-      <c r="P196" s="6"/>
-      <c r="Q196" s="6"/>
-      <c r="R196" s="6"/>
-      <c r="S196" s="6"/>
-      <c r="T196" s="6"/>
-    </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
+      <c r="E195" s="6"/>
+      <c r="F195" s="6"/>
+      <c r="G195" s="6"/>
+      <c r="H195" s="6"/>
+      <c r="I195" s="6"/>
+      <c r="J195" s="6"/>
+      <c r="K195" s="6"/>
+      <c r="L195" s="6"/>
+      <c r="M195" s="6"/>
+      <c r="N195" s="6"/>
+      <c r="O195" s="6"/>
+      <c r="P195" s="6"/>
+      <c r="Q195" s="6"/>
+      <c r="R195" s="6"/>
+      <c r="S195" s="6"/>
+      <c r="T195" s="6"/>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C198" s="3">
+      <c r="C197" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="6" t="s">
+    <row r="198" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B199" s="6"/>
-      <c r="C199" s="6"/>
-      <c r="D199" s="6"/>
-      <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
-      <c r="G199" s="6"/>
-      <c r="H199" s="6"/>
-      <c r="I199" s="6"/>
-      <c r="J199" s="6"/>
-      <c r="K199" s="6"/>
-      <c r="L199" s="6"/>
-      <c r="M199" s="6"/>
-      <c r="N199" s="6"/>
-      <c r="O199" s="6"/>
-      <c r="P199" s="6"/>
-      <c r="Q199" s="6"/>
-      <c r="R199" s="6"/>
-      <c r="S199" s="6"/>
-      <c r="T199" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+      <c r="J198" s="6"/>
+      <c r="K198" s="6"/>
+      <c r="L198" s="6"/>
+      <c r="M198" s="6"/>
+      <c r="N198" s="6"/>
+      <c r="O198" s="6"/>
+      <c r="P198" s="6"/>
+      <c r="Q198" s="6"/>
+      <c r="R198" s="6"/>
+      <c r="S198" s="6"/>
+      <c r="T198" s="6"/>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C201" s="3">
+        <v>40315</v>
+      </c>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C202" s="3">
-        <v>40315</v>
-      </c>
-    </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="A202" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A193:T193"/>
-    <mergeCell ref="A196:T196"/>
-    <mergeCell ref="A199:T199"/>
+    <mergeCell ref="A192:T192"/>
+    <mergeCell ref="A195:T195"/>
+    <mergeCell ref="A198:T198"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B99" r:id="rId1"/>
+    <hyperlink ref="B98" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add version info for 2.5.1 release
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$90</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$96</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -583,6 +583,21 @@
   </si>
   <si>
     <t>Support for solving non-linear models using both NOMAD and the cloud-based NEOS servers (assuming non-negativity currently doesn't work correctly for non-linear NEOS, all variables are assumed positive, not just unconstrained ones)</t>
+  </si>
+  <si>
+    <t>Version 2.5.1 alpha</t>
+  </si>
+  <si>
+    <t>Stability fixes for NOMAD non-linear solver</t>
+  </si>
+  <si>
+    <t>Re-add NEOS non-linear solvers to release with lots of bug fixes.</t>
+  </si>
+  <si>
+    <t>Bug fixes for sensitivity analysis methods.</t>
+  </si>
+  <si>
+    <t>Inclusion of 64-bit CBC with release - appropriate version is selected automatically</t>
   </si>
 </sst>
 </file>
@@ -962,10 +977,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T202"/>
+  <dimension ref="A1:T208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,271 +1038,274 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="1">
-        <v>41810</v>
+        <v>174</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>175</v>
+      </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>169</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>170</v>
+      <c r="A15" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="1">
+        <v>41810</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="1">
-        <v>41324</v>
+      <c r="A17" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>172</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>173</v>
+      </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>169</v>
+      </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>170</v>
+      </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" s="1"/>
+      <c r="A22" s="2"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C23" s="1"/>
+      <c r="A23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="1">
+        <v>41324</v>
+      </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C24" s="1"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C25" s="1"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C26" s="1"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C27" s="1"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C28" s="1"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C29" s="1"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C30" s="1"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C32" s="1"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C33" s="1"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C34" s="1"/>
       <c r="H34" s="5"/>
     </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="H35" s="5"/>
+    </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="1">
-        <v>41211</v>
-      </c>
+      <c r="A36" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>148</v>
-      </c>
+      <c r="A37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="1">
+        <v>41211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C46" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C50" s="1">
         <v>41157</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="1">
-        <v>40963</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,789 +1313,820 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C55" s="1">
-        <v>40882</v>
+        <v>40963</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="1"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>132</v>
-      </c>
-      <c r="C57" s="1"/>
+      <c r="A57" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>142</v>
-      </c>
-      <c r="C58" s="1"/>
+        <v>137</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>133</v>
-      </c>
-      <c r="C59" s="1"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C61" s="1">
-        <v>40877</v>
+        <v>40882</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>129</v>
+      <c r="A63" t="s">
+        <v>132</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>128</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+      <c r="A65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" s="1">
-        <v>40858</v>
-      </c>
+      <c r="A66" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="1"/>
+      <c r="A67" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" s="1">
+        <v>40877</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>120</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>121</v>
-      </c>
+      <c r="A69" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>122</v>
-      </c>
+      <c r="A71" s="2"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>124</v>
+      <c r="A72" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" s="1">
+        <v>40858</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
+      <c r="A73" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C74" s="1">
-        <v>40815</v>
+      <c r="A74" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>102</v>
+      <c r="A75" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>110</v>
-      </c>
+      <c r="A79" s="2"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>111</v>
+      <c r="A80" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" s="1">
+        <v>40815</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>112</v>
+      <c r="A81" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
+      <c r="A88" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C89" s="1">
-        <v>40764</v>
+      <c r="A89" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>96</v>
-      </c>
-      <c r="B92" s="5"/>
+        <v>118</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
+      <c r="A94" s="2"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C95" s="1">
-        <v>40755</v>
+        <v>40764</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C101" s="1">
+        <v>40755</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>89</v>
-      </c>
+      <c r="A126" s="4"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="4"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C129" s="1">
-        <v>40731</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>60</v>
-      </c>
-      <c r="C130" s="1"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C131" s="1"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C132" s="1"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C133" s="1"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C135" s="1">
-        <v>40610</v>
+        <v>40731</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>58</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C138" s="1">
-        <v>40606</v>
-      </c>
+      <c r="A138" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C138" s="1"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>2</v>
-      </c>
+      <c r="A139" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C139" s="1"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>3</v>
+      <c r="A141" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C141" s="1">
+        <v>40610</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" s="1">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B147" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>13</v>
+      <c r="B153" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B155" t="s">
-        <v>15</v>
+      <c r="A155" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>16</v>
+      <c r="B156" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>19</v>
+      <c r="B158" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>18</v>
+      <c r="A159" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>36</v>
+      <c r="A162" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>38</v>
+      <c r="A164" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>22</v>
+      <c r="B165" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>25</v>
+      <c r="B169" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>32</v>
+      <c r="A171" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>27</v>
+      <c r="B172" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B177" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B187" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C187" s="3">
+      <c r="C193" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C191" s="3">
-        <v>40375</v>
-      </c>
-    </row>
-    <row r="192" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B192" s="7"/>
-      <c r="C192" s="7"/>
-      <c r="D192" s="7"/>
-      <c r="E192" s="7"/>
-      <c r="F192" s="7"/>
-      <c r="G192" s="7"/>
-      <c r="H192" s="7"/>
-      <c r="I192" s="7"/>
-      <c r="J192" s="7"/>
-      <c r="K192" s="7"/>
-      <c r="L192" s="7"/>
-      <c r="M192" s="7"/>
-      <c r="N192" s="7"/>
-      <c r="O192" s="7"/>
-      <c r="P192" s="7"/>
-      <c r="Q192" s="7"/>
-      <c r="R192" s="7"/>
-      <c r="S192" s="7"/>
-      <c r="T192" s="7"/>
-    </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C194" s="3">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="195" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B195" s="6"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
-      <c r="G195" s="6"/>
-      <c r="H195" s="6"/>
-      <c r="I195" s="6"/>
-      <c r="J195" s="6"/>
-      <c r="K195" s="6"/>
-      <c r="L195" s="6"/>
-      <c r="M195" s="6"/>
-      <c r="N195" s="6"/>
-      <c r="O195" s="6"/>
-      <c r="P195" s="6"/>
-      <c r="Q195" s="6"/>
-      <c r="R195" s="6"/>
-      <c r="S195" s="6"/>
-      <c r="T195" s="6"/>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C197" s="3">
+        <v>40375</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B198" s="7"/>
+      <c r="C198" s="7"/>
+      <c r="D198" s="7"/>
+      <c r="E198" s="7"/>
+      <c r="F198" s="7"/>
+      <c r="G198" s="7"/>
+      <c r="H198" s="7"/>
+      <c r="I198" s="7"/>
+      <c r="J198" s="7"/>
+      <c r="K198" s="7"/>
+      <c r="L198" s="7"/>
+      <c r="M198" s="7"/>
+      <c r="N198" s="7"/>
+      <c r="O198" s="7"/>
+      <c r="P198" s="7"/>
+      <c r="Q198" s="7"/>
+      <c r="R198" s="7"/>
+      <c r="S198" s="7"/>
+      <c r="T198" s="7"/>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C197" s="3">
+      <c r="C200" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="6" t="s">
+    <row r="201" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+      <c r="D201" s="6"/>
+      <c r="E201" s="6"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+      <c r="J201" s="6"/>
+      <c r="K201" s="6"/>
+      <c r="L201" s="6"/>
+      <c r="M201" s="6"/>
+      <c r="N201" s="6"/>
+      <c r="O201" s="6"/>
+      <c r="P201" s="6"/>
+      <c r="Q201" s="6"/>
+      <c r="R201" s="6"/>
+      <c r="S201" s="6"/>
+      <c r="T201" s="6"/>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C203" s="3">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B198" s="6"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="6"/>
-      <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
-      <c r="G198" s="6"/>
-      <c r="H198" s="6"/>
-      <c r="I198" s="6"/>
-      <c r="J198" s="6"/>
-      <c r="K198" s="6"/>
-      <c r="L198" s="6"/>
-      <c r="M198" s="6"/>
-      <c r="N198" s="6"/>
-      <c r="O198" s="6"/>
-      <c r="P198" s="6"/>
-      <c r="Q198" s="6"/>
-      <c r="R198" s="6"/>
-      <c r="S198" s="6"/>
-      <c r="T198" s="6"/>
-    </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
+      <c r="B204" s="6"/>
+      <c r="C204" s="6"/>
+      <c r="D204" s="6"/>
+      <c r="E204" s="6"/>
+      <c r="F204" s="6"/>
+      <c r="G204" s="6"/>
+      <c r="H204" s="6"/>
+      <c r="I204" s="6"/>
+      <c r="J204" s="6"/>
+      <c r="K204" s="6"/>
+      <c r="L204" s="6"/>
+      <c r="M204" s="6"/>
+      <c r="N204" s="6"/>
+      <c r="O204" s="6"/>
+      <c r="P204" s="6"/>
+      <c r="Q204" s="6"/>
+      <c r="R204" s="6"/>
+      <c r="S204" s="6"/>
+      <c r="T204" s="6"/>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C201" s="3">
+      <c r="C207" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A192:T192"/>
-    <mergeCell ref="A195:T195"/>
     <mergeCell ref="A198:T198"/>
+    <mergeCell ref="A201:T201"/>
+    <mergeCell ref="A204:T204"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B98" r:id="rId1"/>
+    <hyperlink ref="B104" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set release info for 2.5.2
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$96</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$100</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="182">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -598,6 +598,15 @@
   </si>
   <si>
     <t>Inclusion of 64-bit CBC with release - appropriate version is selected automatically</t>
+  </si>
+  <si>
+    <t>Version 2.5.2 alpha</t>
+  </si>
+  <si>
+    <t>Fix memory bug causing Excel 2013 to crash when using NOMAD</t>
+  </si>
+  <si>
+    <t>Non-linear NEOS bug fixes</t>
   </si>
 </sst>
 </file>
@@ -977,10 +986,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T208"/>
+  <dimension ref="A1:T212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,600 +1047,604 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C15" s="1">
-        <v>41810</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>176</v>
+      </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>172</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>173</v>
+      <c r="A19" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="1">
+        <v>41810</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="1">
-        <v>41324</v>
+      <c r="A23" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>169</v>
+      </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>170</v>
+      </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="1"/>
+      <c r="A26" s="2"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="1"/>
+      <c r="A27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="1">
+        <v>41324</v>
+      </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C28" s="1"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C29" s="1"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C30" s="1"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C31" s="1"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C32" s="1"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C33" s="1"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C34" s="1"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C35" s="1"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C36" s="1"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C37" s="1"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C38" s="1"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C39" s="1"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C40" s="1"/>
       <c r="H40" s="5"/>
     </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="H41" s="5"/>
+    </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C42" s="1">
-        <v>41211</v>
-      </c>
+      <c r="A42" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>148</v>
-      </c>
+      <c r="A43" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+        <v>163</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="H44" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C46" s="1">
-        <v>41176</v>
+        <v>41211</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="1">
+        <v>41176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C54" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C55" s="1">
-        <v>40963</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="1">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C61" s="1">
-        <v>40882</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="1"/>
+        <v>137</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="1">
+        <v>40882</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>142</v>
-      </c>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>133</v>
-      </c>
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C67" s="1">
-        <v>40877</v>
-      </c>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" s="1">
-        <v>40858</v>
-      </c>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>121</v>
-      </c>
+      <c r="A75" s="2"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>123</v>
+      <c r="A76" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="1">
+        <v>40858</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>122</v>
-      </c>
+      <c r="A77" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
+      <c r="A79" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C80" s="1">
-        <v>40815</v>
+      <c r="A80" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>102</v>
+      <c r="A81" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>105</v>
-      </c>
+      <c r="A83" s="2"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>106</v>
+      <c r="A84" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" s="1">
+        <v>40815</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>110</v>
+      <c r="A85" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
+      <c r="A94" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C95" s="1">
-        <v>40764</v>
+      <c r="A95" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" s="1">
+        <v>40764</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>96</v>
-      </c>
-      <c r="B98" s="5"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C101" s="1">
-        <v>40755</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>65</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B102" s="5"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="A104" s="4"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>67</v>
+      <c r="A105" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C105" s="1">
+        <v>40755</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
+      <c r="A106" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>69</v>
+      <c r="B108" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>70</v>
+      <c r="B109" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>71</v>
-      </c>
+      <c r="A110" s="4"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
+      <c r="A113" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>76</v>
+      <c r="A116" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -1639,60 +1652,60 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>80</v>
-      </c>
+      <c r="A121" s="4"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>81</v>
+      <c r="A122" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>82</v>
+      <c r="A123" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1700,433 +1713,451 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="2"/>
+      <c r="A134" s="4"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C135" s="1">
-        <v>40731</v>
+      <c r="A135" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C139" s="1">
+        <v>40731</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>60</v>
       </c>
-      <c r="C136" s="1"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="4" t="s">
+      <c r="C140" s="1"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C137" s="1"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="4" t="s">
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C138" s="1"/>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="4" t="s">
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C139" s="1"/>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="C143" s="1"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C145" s="1">
         <v>40610</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C148" s="1">
         <v>40606</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>16</v>
+      <c r="B162" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>17</v>
+      <c r="A163" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>19</v>
+      <c r="B164" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
-        <v>20</v>
+      <c r="A166" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>36</v>
+      <c r="A168" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>22</v>
+      <c r="B171" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>27</v>
+      <c r="B178" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>28</v>
+      <c r="A179" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>54</v>
+      <c r="B180" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="B187" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>40</v>
+      <c r="A188" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B191" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A193" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C193" s="3">
-        <v>40407</v>
-      </c>
-    </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C197" s="3">
+        <v>40407</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C197" s="3">
+      <c r="C201" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="6" t="s">
+    <row r="202" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B198" s="7"/>
-      <c r="C198" s="7"/>
-      <c r="D198" s="7"/>
-      <c r="E198" s="7"/>
-      <c r="F198" s="7"/>
-      <c r="G198" s="7"/>
-      <c r="H198" s="7"/>
-      <c r="I198" s="7"/>
-      <c r="J198" s="7"/>
-      <c r="K198" s="7"/>
-      <c r="L198" s="7"/>
-      <c r="M198" s="7"/>
-      <c r="N198" s="7"/>
-      <c r="O198" s="7"/>
-      <c r="P198" s="7"/>
-      <c r="Q198" s="7"/>
-      <c r="R198" s="7"/>
-      <c r="S198" s="7"/>
-      <c r="T198" s="7"/>
-    </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
+      <c r="B202" s="7"/>
+      <c r="C202" s="7"/>
+      <c r="D202" s="7"/>
+      <c r="E202" s="7"/>
+      <c r="F202" s="7"/>
+      <c r="G202" s="7"/>
+      <c r="H202" s="7"/>
+      <c r="I202" s="7"/>
+      <c r="J202" s="7"/>
+      <c r="K202" s="7"/>
+      <c r="L202" s="7"/>
+      <c r="M202" s="7"/>
+      <c r="N202" s="7"/>
+      <c r="O202" s="7"/>
+      <c r="P202" s="7"/>
+      <c r="Q202" s="7"/>
+      <c r="R202" s="7"/>
+      <c r="S202" s="7"/>
+      <c r="T202" s="7"/>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C200" s="3">
+      <c r="C204" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="6" t="s">
+    <row r="205" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B201" s="6"/>
-      <c r="C201" s="6"/>
-      <c r="D201" s="6"/>
-      <c r="E201" s="6"/>
-      <c r="F201" s="6"/>
-      <c r="G201" s="6"/>
-      <c r="H201" s="6"/>
-      <c r="I201" s="6"/>
-      <c r="J201" s="6"/>
-      <c r="K201" s="6"/>
-      <c r="L201" s="6"/>
-      <c r="M201" s="6"/>
-      <c r="N201" s="6"/>
-      <c r="O201" s="6"/>
-      <c r="P201" s="6"/>
-      <c r="Q201" s="6"/>
-      <c r="R201" s="6"/>
-      <c r="S201" s="6"/>
-      <c r="T201" s="6"/>
-    </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C203" s="3">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="204" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B204" s="6"/>
-      <c r="C204" s="6"/>
-      <c r="D204" s="6"/>
-      <c r="E204" s="6"/>
-      <c r="F204" s="6"/>
-      <c r="G204" s="6"/>
-      <c r="H204" s="6"/>
-      <c r="I204" s="6"/>
-      <c r="J204" s="6"/>
-      <c r="K204" s="6"/>
-      <c r="L204" s="6"/>
-      <c r="M204" s="6"/>
-      <c r="N204" s="6"/>
-      <c r="O204" s="6"/>
-      <c r="P204" s="6"/>
-      <c r="Q204" s="6"/>
-      <c r="R204" s="6"/>
-      <c r="S204" s="6"/>
-      <c r="T204" s="6"/>
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
+      <c r="E205" s="6"/>
+      <c r="F205" s="6"/>
+      <c r="G205" s="6"/>
+      <c r="H205" s="6"/>
+      <c r="I205" s="6"/>
+      <c r="J205" s="6"/>
+      <c r="K205" s="6"/>
+      <c r="L205" s="6"/>
+      <c r="M205" s="6"/>
+      <c r="N205" s="6"/>
+      <c r="O205" s="6"/>
+      <c r="P205" s="6"/>
+      <c r="Q205" s="6"/>
+      <c r="R205" s="6"/>
+      <c r="S205" s="6"/>
+      <c r="T205" s="6"/>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C207" s="3">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="6"/>
+      <c r="E208" s="6"/>
+      <c r="F208" s="6"/>
+      <c r="G208" s="6"/>
+      <c r="H208" s="6"/>
+      <c r="I208" s="6"/>
+      <c r="J208" s="6"/>
+      <c r="K208" s="6"/>
+      <c r="L208" s="6"/>
+      <c r="M208" s="6"/>
+      <c r="N208" s="6"/>
+      <c r="O208" s="6"/>
+      <c r="P208" s="6"/>
+      <c r="Q208" s="6"/>
+      <c r="R208" s="6"/>
+      <c r="S208" s="6"/>
+      <c r="T208" s="6"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C207" s="3">
+      <c r="C211" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A198:T198"/>
-    <mergeCell ref="A201:T201"/>
-    <mergeCell ref="A204:T204"/>
+    <mergeCell ref="A202:T202"/>
+    <mergeCell ref="A205:T205"/>
+    <mergeCell ref="A208:T208"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B104" r:id="rId1"/>
+    <hyperlink ref="B108" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add info for 2.5.3 release
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$100</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$103</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>Non-linear NEOS bug fixes</t>
+  </si>
+  <si>
+    <t>Version 2.5.3 alpha</t>
+  </si>
+  <si>
+    <t>Add support for NOMAD in 64-bit Office.</t>
   </si>
 </sst>
 </file>
@@ -986,10 +992,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T212"/>
+  <dimension ref="A1:T215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,1063 +1053,1047 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>176</v>
+      <c r="A16" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4" t="s">
+        <v>178</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="1">
-        <v>41810</v>
+      <c r="A19" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>177</v>
+      </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="A21" s="2"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>172</v>
+      <c r="A22" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="1">
+        <v>41810</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C23" s="1"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C27" s="1">
-        <v>41324</v>
+      <c r="A27" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>170</v>
+      </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="1"/>
+      <c r="A29" s="2"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" s="1"/>
+      <c r="A30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="1">
+        <v>41324</v>
+      </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C31" s="1"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C32" s="1"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C33" s="1"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C35" s="1"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C36" s="1"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C37" s="1"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C38" s="1"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C39" s="1"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C40" s="1"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" s="1"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C42" s="1"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C43" s="1"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C44" s="1"/>
       <c r="H44" s="5"/>
     </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="H45" s="5"/>
+    </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C49" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C53" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C54" s="1">
-        <v>41157</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="1">
+        <v>41157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C62" s="1">
         <v>40963</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
+      <c r="A64" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C65" s="1">
-        <v>40882</v>
+      <c r="A65" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" s="1"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="1"/>
+      <c r="A67" s="2"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>142</v>
-      </c>
-      <c r="C68" s="1"/>
+      <c r="A68" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="1">
+        <v>40882</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
+      <c r="A70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C71" s="1">
-        <v>40877</v>
-      </c>
+      <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>127</v>
       </c>
-      <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C79" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>123</v>
-      </c>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C87" s="1">
         <v>40815</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
+      <c r="A98" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C99" s="1">
-        <v>40764</v>
+      <c r="A99" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>94</v>
-      </c>
+      <c r="A101" s="2"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>96</v>
-      </c>
-      <c r="B102" s="5"/>
+      <c r="A102" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C102" s="1">
+        <v>40764</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
+      <c r="A104" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C105" s="1">
-        <v>40755</v>
-      </c>
+      <c r="A105" t="s">
+        <v>96</v>
+      </c>
+      <c r="B105" s="5"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C108" s="1">
+        <v>40755</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="5" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>70</v>
-      </c>
+      <c r="A113" s="4"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="4"/>
+      <c r="A117" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>76</v>
-      </c>
+      <c r="A120" s="4"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
+      <c r="A121" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="4"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2"/>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C139" s="1">
-        <v>40731</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C142" s="1">
+        <v>40731</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>60</v>
       </c>
-      <c r="C140" s="1"/>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="4" t="s">
+      <c r="C143" s="1"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C141" s="1"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="4" t="s">
+      <c r="C144" s="1"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C142" s="1"/>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="4" t="s">
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C143" s="1"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C145" s="1">
-        <v>40610</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>58</v>
-      </c>
+      <c r="C146" s="1"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C148" s="1">
-        <v>40606</v>
+        <v>40610</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>3</v>
+      <c r="A151" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" s="1">
+        <v>40606</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B155" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>10</v>
+      <c r="B159" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>24</v>
+      <c r="A162" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>13</v>
+      <c r="B163" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>19</v>
+      <c r="B168" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
-        <v>18</v>
+      <c r="A169" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>29</v>
+      <c r="A171" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>22</v>
+      <c r="B175" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>31</v>
+      <c r="A178" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>25</v>
+      <c r="B179" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B191" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B194" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C197" s="3">
+      <c r="C200" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C201" s="3">
-        <v>40375</v>
-      </c>
-    </row>
-    <row r="202" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B202" s="7"/>
-      <c r="C202" s="7"/>
-      <c r="D202" s="7"/>
-      <c r="E202" s="7"/>
-      <c r="F202" s="7"/>
-      <c r="G202" s="7"/>
-      <c r="H202" s="7"/>
-      <c r="I202" s="7"/>
-      <c r="J202" s="7"/>
-      <c r="K202" s="7"/>
-      <c r="L202" s="7"/>
-      <c r="M202" s="7"/>
-      <c r="N202" s="7"/>
-      <c r="O202" s="7"/>
-      <c r="P202" s="7"/>
-      <c r="Q202" s="7"/>
-      <c r="R202" s="7"/>
-      <c r="S202" s="7"/>
-      <c r="T202" s="7"/>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C204" s="3">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="205" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40375</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B205" s="6"/>
-      <c r="C205" s="6"/>
-      <c r="D205" s="6"/>
-      <c r="E205" s="6"/>
-      <c r="F205" s="6"/>
-      <c r="G205" s="6"/>
-      <c r="H205" s="6"/>
-      <c r="I205" s="6"/>
-      <c r="J205" s="6"/>
-      <c r="K205" s="6"/>
-      <c r="L205" s="6"/>
-      <c r="M205" s="6"/>
-      <c r="N205" s="6"/>
-      <c r="O205" s="6"/>
-      <c r="P205" s="6"/>
-      <c r="Q205" s="6"/>
-      <c r="R205" s="6"/>
-      <c r="S205" s="6"/>
-      <c r="T205" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="B205" s="7"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
+      <c r="G205" s="7"/>
+      <c r="H205" s="7"/>
+      <c r="I205" s="7"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="M205" s="7"/>
+      <c r="N205" s="7"/>
+      <c r="O205" s="7"/>
+      <c r="P205" s="7"/>
+      <c r="Q205" s="7"/>
+      <c r="R205" s="7"/>
+      <c r="S205" s="7"/>
+      <c r="T205" s="7"/>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
@@ -2115,7 +2105,7 @@
     </row>
     <row r="208" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
@@ -2137,27 +2127,59 @@
       <c r="S208" s="6"/>
       <c r="T208" s="6"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C210" s="3">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
+      <c r="D211" s="6"/>
+      <c r="E211" s="6"/>
+      <c r="F211" s="6"/>
+      <c r="G211" s="6"/>
+      <c r="H211" s="6"/>
+      <c r="I211" s="6"/>
+      <c r="J211" s="6"/>
+      <c r="K211" s="6"/>
+      <c r="L211" s="6"/>
+      <c r="M211" s="6"/>
+      <c r="N211" s="6"/>
+      <c r="O211" s="6"/>
+      <c r="P211" s="6"/>
+      <c r="Q211" s="6"/>
+      <c r="R211" s="6"/>
+      <c r="S211" s="6"/>
+      <c r="T211" s="6"/>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C211" s="3">
+      <c r="C214" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A202:T202"/>
     <mergeCell ref="A205:T205"/>
     <mergeCell ref="A208:T208"/>
+    <mergeCell ref="A211:T211"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B108" r:id="rId1"/>
+    <hyperlink ref="B111" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepare version info for release
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$103</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$106</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="186">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -613,6 +613,12 @@
   </si>
   <si>
     <t>Add support for NOMAD in 64-bit Office.</t>
+  </si>
+  <si>
+    <t>Version 2.5.4 alpha</t>
+  </si>
+  <si>
+    <t>NOMAD bug fixes for when errors are encountered</t>
   </si>
 </sst>
 </file>
@@ -992,10 +998,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T215"/>
+  <dimension ref="A1:T218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,13 +1059,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -1069,1063 +1075,1047 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>178</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>176</v>
+      <c r="A19" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4" t="s">
+        <v>178</v>
+      </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="1">
-        <v>41810</v>
+      <c r="A22" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>177</v>
+      </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>172</v>
+      <c r="A25" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="1">
+        <v>41810</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" s="1">
-        <v>41324</v>
+      <c r="A30" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>170</v>
+      </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C32" s="1"/>
+      <c r="A32" s="2"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C33" s="1"/>
+      <c r="A33" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" s="1">
+        <v>41324</v>
+      </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C34" s="1"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C35" s="1"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C36" s="1"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C37" s="1"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C38" s="1"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C39" s="1"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C40" s="1"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C41" s="1"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C42" s="1"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C43" s="1"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C45" s="1"/>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="1"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C47" s="1"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C52" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C56" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C60" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C65" s="1">
         <v>40963</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
+      <c r="A67" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C68" s="1">
-        <v>40882</v>
+      <c r="A68" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" s="1"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>132</v>
-      </c>
-      <c r="C70" s="1"/>
+      <c r="A70" s="2"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="1"/>
+      <c r="A71" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C71" s="1">
+        <v>40882</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
+      <c r="A73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="1">
-        <v>40877</v>
-      </c>
+      <c r="A74" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>127</v>
       </c>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C82" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>123</v>
-      </c>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C90" s="1">
         <v>40815</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
+      <c r="A101" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C102" s="1">
-        <v>40764</v>
+      <c r="A102" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>94</v>
-      </c>
+      <c r="A104" s="2"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>96</v>
-      </c>
-      <c r="B105" s="5"/>
+      <c r="A105" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C105" s="1">
+        <v>40764</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
+      <c r="A107" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C108" s="1">
-        <v>40755</v>
-      </c>
+      <c r="A108" t="s">
+        <v>96</v>
+      </c>
+      <c r="B108" s="5"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C111" s="1">
+        <v>40755</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="5" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>70</v>
-      </c>
+      <c r="A116" s="4"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
+      <c r="A120" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>76</v>
-      </c>
+      <c r="A123" s="4"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
+      <c r="A124" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="4"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="4"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="4"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="2"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C145" s="1">
         <v>40731</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>60</v>
       </c>
-      <c r="C143" s="1"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="4" t="s">
+      <c r="C146" s="1"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C144" s="1"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="4" t="s">
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C145" s="1"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
+      <c r="C148" s="1"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C146" s="1"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C148" s="1">
-        <v>40610</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>58</v>
-      </c>
+      <c r="C149" s="1"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C151" s="1">
-        <v>40606</v>
+        <v>40610</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>3</v>
+      <c r="A154" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" s="1">
+        <v>40606</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>10</v>
+      <c r="B162" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>24</v>
+      <c r="A165" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>13</v>
+      <c r="B166" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>19</v>
+      <c r="B171" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>18</v>
+      <c r="A172" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>29</v>
+      <c r="A174" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>22</v>
+      <c r="B178" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>31</v>
+      <c r="A181" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>25</v>
+      <c r="B182" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B194" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B197" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C200" s="3">
+      <c r="C203" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C204" s="3">
-        <v>40375</v>
-      </c>
-    </row>
-    <row r="205" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B205" s="7"/>
-      <c r="C205" s="7"/>
-      <c r="D205" s="7"/>
-      <c r="E205" s="7"/>
-      <c r="F205" s="7"/>
-      <c r="G205" s="7"/>
-      <c r="H205" s="7"/>
-      <c r="I205" s="7"/>
-      <c r="J205" s="7"/>
-      <c r="K205" s="7"/>
-      <c r="L205" s="7"/>
-      <c r="M205" s="7"/>
-      <c r="N205" s="7"/>
-      <c r="O205" s="7"/>
-      <c r="P205" s="7"/>
-      <c r="Q205" s="7"/>
-      <c r="R205" s="7"/>
-      <c r="S205" s="7"/>
-      <c r="T205" s="7"/>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C207" s="3">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="208" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40375</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B208" s="6"/>
-      <c r="C208" s="6"/>
-      <c r="D208" s="6"/>
-      <c r="E208" s="6"/>
-      <c r="F208" s="6"/>
-      <c r="G208" s="6"/>
-      <c r="H208" s="6"/>
-      <c r="I208" s="6"/>
-      <c r="J208" s="6"/>
-      <c r="K208" s="6"/>
-      <c r="L208" s="6"/>
-      <c r="M208" s="6"/>
-      <c r="N208" s="6"/>
-      <c r="O208" s="6"/>
-      <c r="P208" s="6"/>
-      <c r="Q208" s="6"/>
-      <c r="R208" s="6"/>
-      <c r="S208" s="6"/>
-      <c r="T208" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="B208" s="7"/>
+      <c r="C208" s="7"/>
+      <c r="D208" s="7"/>
+      <c r="E208" s="7"/>
+      <c r="F208" s="7"/>
+      <c r="G208" s="7"/>
+      <c r="H208" s="7"/>
+      <c r="I208" s="7"/>
+      <c r="J208" s="7"/>
+      <c r="K208" s="7"/>
+      <c r="L208" s="7"/>
+      <c r="M208" s="7"/>
+      <c r="N208" s="7"/>
+      <c r="O208" s="7"/>
+      <c r="P208" s="7"/>
+      <c r="Q208" s="7"/>
+      <c r="R208" s="7"/>
+      <c r="S208" s="7"/>
+      <c r="T208" s="7"/>
     </row>
     <row r="210" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
@@ -2137,7 +2127,7 @@
     </row>
     <row r="211" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
@@ -2159,27 +2149,59 @@
       <c r="S211" s="6"/>
       <c r="T211" s="6"/>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
+    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C213" s="3">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="E214" s="6"/>
+      <c r="F214" s="6"/>
+      <c r="G214" s="6"/>
+      <c r="H214" s="6"/>
+      <c r="I214" s="6"/>
+      <c r="J214" s="6"/>
+      <c r="K214" s="6"/>
+      <c r="L214" s="6"/>
+      <c r="M214" s="6"/>
+      <c r="N214" s="6"/>
+      <c r="O214" s="6"/>
+      <c r="P214" s="6"/>
+      <c r="Q214" s="6"/>
+      <c r="R214" s="6"/>
+      <c r="S214" s="6"/>
+      <c r="T214" s="6"/>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C214" s="3">
+      <c r="C217" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A205:T205"/>
     <mergeCell ref="A208:T208"/>
     <mergeCell ref="A211:T211"/>
+    <mergeCell ref="A214:T214"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B111" r:id="rId1"/>
+    <hyperlink ref="B114" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepare changelog for v2.6
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jack\Dropbox\Scratch\OpenSolverNew\OpenSolver2.4\OpenSolver Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Dropbox (Personal)\Scratch\OpenSolver\OpenSolver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$106</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$115</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="194">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -619,6 +619,30 @@
   </si>
   <si>
     <t>NOMAD bug fixes for when errors are encountered</t>
+  </si>
+  <si>
+    <t>Version 2.6</t>
+  </si>
+  <si>
+    <t>Resolve bugs introduced by system-locale settings</t>
+  </si>
+  <si>
+    <t>NEOS solvers write AMPL files to disk before sending to NEOS. These can be used to run the model locally</t>
+  </si>
+  <si>
+    <t>Upgrade NOMAD to v3.6.2</t>
+  </si>
+  <si>
+    <t>Add support for Office 2011 on Mac - nearly all features supported</t>
+  </si>
+  <si>
+    <t>Add support for local COIN-OR non-linear solvers</t>
+  </si>
+  <si>
+    <t>Bugfixes for non-linear NOMAD solver</t>
+  </si>
+  <si>
+    <t>Bugfixes for NEOS solvers</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1022,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T218"/>
+  <dimension ref="A1:T227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,697 +1083,706 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>182</v>
+      <c r="A12" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>179</v>
+      <c r="A15" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>181</v>
-      </c>
+      <c r="A17" s="2"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>174</v>
+      <c r="A19" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="A20" s="2"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>178</v>
+      <c r="A21" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="A23" s="2"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C25" s="1">
-        <v>41810</v>
+      <c r="A25" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>181</v>
+      </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="A27" s="2"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>172</v>
+      <c r="A28" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="1">
-        <v>41324</v>
-      </c>
+      <c r="A33" s="2"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="1"/>
+      <c r="A34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="1">
+        <v>41810</v>
+      </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C35" s="1"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" s="1"/>
+        <v>168</v>
+      </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="1"/>
+        <v>172</v>
+      </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>173</v>
+      </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>169</v>
+      </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C40" s="1"/>
+        <v>170</v>
+      </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C41" s="1"/>
+      <c r="A41" s="2"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" s="1"/>
+      <c r="A42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="1">
+        <v>41324</v>
+      </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C43" s="1"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C44" s="1"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C45" s="1"/>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C46" s="1"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C47" s="1"/>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C48" s="1"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C49" s="1"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C50" s="1"/>
       <c r="H50" s="5"/>
     </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="H51" s="5"/>
+    </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="1">
-        <v>41211</v>
-      </c>
+      <c r="A52" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>148</v>
-      </c>
+      <c r="A53" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>147</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
+      <c r="A55" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C56" s="1">
-        <v>41176</v>
-      </c>
+      <c r="A56" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>144</v>
-      </c>
+      <c r="A57" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>145</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C60" s="1">
-        <v>41157</v>
-      </c>
+      <c r="A59" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="H59" s="5"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>140</v>
+      <c r="A61" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="1">
+        <v>41211</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>141</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
+      <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C65" s="1">
-        <v>40963</v>
+        <v>41176</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>137</v>
-      </c>
+      <c r="A68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>138</v>
+      <c r="A69" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="1">
+        <v>41157</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
+      <c r="A70" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C71" s="1">
-        <v>40882</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>131</v>
-      </c>
-      <c r="C72" s="1"/>
+      <c r="A71" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>132</v>
-      </c>
-      <c r="C73" s="1"/>
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>142</v>
-      </c>
-      <c r="C74" s="1"/>
+      <c r="A74" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="1">
+        <v>40963</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>133</v>
-      </c>
-      <c r="C75" s="1"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
+      <c r="A76" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C77" s="1">
-        <v>40877</v>
+      <c r="A77" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="1"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" s="1"/>
+      <c r="A79" s="2"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>128</v>
+      <c r="A80" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="1">
+        <v>40882</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
+      <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C82" s="1">
-        <v>40858</v>
-      </c>
+      <c r="A82" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>125</v>
+      <c r="A83" t="s">
+        <v>142</v>
       </c>
       <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>121</v>
-      </c>
+      <c r="A85" s="2"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>123</v>
+      <c r="A86" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C86" s="1">
+        <v>40877</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>122</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>124</v>
-      </c>
+      <c r="A88" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
+      <c r="A89" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C90" s="1">
-        <v>40815</v>
-      </c>
+      <c r="A90" s="2"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>102</v>
+      <c r="A91" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C91" s="1">
+        <v>40858</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>104</v>
-      </c>
+      <c r="A92" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>113</v>
-      </c>
+      <c r="A98" s="2"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>114</v>
+      <c r="A99" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="1">
+        <v>40815</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>115</v>
+      <c r="A100" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
+      <c r="A104" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C105" s="1">
-        <v>40764</v>
+      <c r="A105" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>96</v>
-      </c>
-      <c r="B108" s="5"/>
+        <v>114</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
+      <c r="A110" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C111" s="1">
-        <v>40755</v>
+      <c r="A111" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C114" s="1">
+        <v>40764</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>96</v>
+      </c>
+      <c r="B117" s="5"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C120" s="1">
+        <v>40755</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="5" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="4"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="4"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
-        <v>79</v>
+      <c r="A130" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>80</v>
+      <c r="A131" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>81</v>
-      </c>
+      <c r="A132" s="4"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
-        <v>82</v>
+      <c r="A133" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
-        <v>83</v>
+      <c r="A134" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -1757,451 +1790,494 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>87</v>
+      <c r="B139" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="4"/>
+      <c r="B140" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>88</v>
+      <c r="B141" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>89</v>
+      <c r="B142" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>90</v>
+      <c r="B143" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="2"/>
+      <c r="B144" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C145" s="1">
-        <v>40731</v>
-      </c>
+      <c r="A145" s="4"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>60</v>
-      </c>
-      <c r="C146" s="1"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C147" s="1"/>
+      <c r="A147" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C148" s="1"/>
+      <c r="A148" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C149" s="1"/>
+      <c r="A149" s="4"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C151" s="1">
-        <v>40610</v>
+      <c r="A151" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>58</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C154" s="1">
-        <v>40606</v>
+        <v>40731</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>60</v>
+      </c>
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C158" s="1"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C160" s="1">
+        <v>40610</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" s="1">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>36</v>
+      <c r="A178" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
-        <v>30</v>
+      <c r="A183" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>25</v>
+      <c r="B185" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>27</v>
+      <c r="B188" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B206" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C203" s="3">
+      <c r="C212" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
+    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C207" s="3">
+      <c r="C216" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="6" t="s">
+    <row r="217" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B208" s="7"/>
-      <c r="C208" s="7"/>
-      <c r="D208" s="7"/>
-      <c r="E208" s="7"/>
-      <c r="F208" s="7"/>
-      <c r="G208" s="7"/>
-      <c r="H208" s="7"/>
-      <c r="I208" s="7"/>
-      <c r="J208" s="7"/>
-      <c r="K208" s="7"/>
-      <c r="L208" s="7"/>
-      <c r="M208" s="7"/>
-      <c r="N208" s="7"/>
-      <c r="O208" s="7"/>
-      <c r="P208" s="7"/>
-      <c r="Q208" s="7"/>
-      <c r="R208" s="7"/>
-      <c r="S208" s="7"/>
-      <c r="T208" s="7"/>
-    </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
+      <c r="B217" s="7"/>
+      <c r="C217" s="7"/>
+      <c r="D217" s="7"/>
+      <c r="E217" s="7"/>
+      <c r="F217" s="7"/>
+      <c r="G217" s="7"/>
+      <c r="H217" s="7"/>
+      <c r="I217" s="7"/>
+      <c r="J217" s="7"/>
+      <c r="K217" s="7"/>
+      <c r="L217" s="7"/>
+      <c r="M217" s="7"/>
+      <c r="N217" s="7"/>
+      <c r="O217" s="7"/>
+      <c r="P217" s="7"/>
+      <c r="Q217" s="7"/>
+      <c r="R217" s="7"/>
+      <c r="S217" s="7"/>
+      <c r="T217" s="7"/>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C210" s="3">
+      <c r="C219" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="6" t="s">
+    <row r="220" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B211" s="6"/>
-      <c r="C211" s="6"/>
-      <c r="D211" s="6"/>
-      <c r="E211" s="6"/>
-      <c r="F211" s="6"/>
-      <c r="G211" s="6"/>
-      <c r="H211" s="6"/>
-      <c r="I211" s="6"/>
-      <c r="J211" s="6"/>
-      <c r="K211" s="6"/>
-      <c r="L211" s="6"/>
-      <c r="M211" s="6"/>
-      <c r="N211" s="6"/>
-      <c r="O211" s="6"/>
-      <c r="P211" s="6"/>
-      <c r="Q211" s="6"/>
-      <c r="R211" s="6"/>
-      <c r="S211" s="6"/>
-      <c r="T211" s="6"/>
-    </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+      <c r="D220" s="6"/>
+      <c r="E220" s="6"/>
+      <c r="F220" s="6"/>
+      <c r="G220" s="6"/>
+      <c r="H220" s="6"/>
+      <c r="I220" s="6"/>
+      <c r="J220" s="6"/>
+      <c r="K220" s="6"/>
+      <c r="L220" s="6"/>
+      <c r="M220" s="6"/>
+      <c r="N220" s="6"/>
+      <c r="O220" s="6"/>
+      <c r="P220" s="6"/>
+      <c r="Q220" s="6"/>
+      <c r="R220" s="6"/>
+      <c r="S220" s="6"/>
+      <c r="T220" s="6"/>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C213" s="3">
+      <c r="C222" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="6" t="s">
+    <row r="223" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B214" s="6"/>
-      <c r="C214" s="6"/>
-      <c r="D214" s="6"/>
-      <c r="E214" s="6"/>
-      <c r="F214" s="6"/>
-      <c r="G214" s="6"/>
-      <c r="H214" s="6"/>
-      <c r="I214" s="6"/>
-      <c r="J214" s="6"/>
-      <c r="K214" s="6"/>
-      <c r="L214" s="6"/>
-      <c r="M214" s="6"/>
-      <c r="N214" s="6"/>
-      <c r="O214" s="6"/>
-      <c r="P214" s="6"/>
-      <c r="Q214" s="6"/>
-      <c r="R214" s="6"/>
-      <c r="S214" s="6"/>
-      <c r="T214" s="6"/>
-    </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
+      <c r="D223" s="6"/>
+      <c r="E223" s="6"/>
+      <c r="F223" s="6"/>
+      <c r="G223" s="6"/>
+      <c r="H223" s="6"/>
+      <c r="I223" s="6"/>
+      <c r="J223" s="6"/>
+      <c r="K223" s="6"/>
+      <c r="L223" s="6"/>
+      <c r="M223" s="6"/>
+      <c r="N223" s="6"/>
+      <c r="O223" s="6"/>
+      <c r="P223" s="6"/>
+      <c r="Q223" s="6"/>
+      <c r="R223" s="6"/>
+      <c r="S223" s="6"/>
+      <c r="T223" s="6"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C217" s="3">
+      <c r="C226" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A208:T208"/>
-    <mergeCell ref="A211:T211"/>
-    <mergeCell ref="A214:T214"/>
+    <mergeCell ref="A217:T217"/>
+    <mergeCell ref="A220:T220"/>
+    <mergeCell ref="A223:T223"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B114" r:id="rId1"/>
+    <hyperlink ref="B123" r:id="rId1"/>
     <hyperlink ref="H7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepare version info for 2.6 release
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:T227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,6 +1084,9 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>186</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41911</v>
       </c>
       <c r="H9" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update changelog for 2.6.1
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Dropbox\Scratch\OpenSolver\OpenSolver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Dropbox (Personal)\Scratch\OpenSolver\OpenSolver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$115</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$127</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -34,12 +34,12 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="203">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -332,27 +332,12 @@
     <t>We now pass the solve options (such as tolerance) to CBC both when solving the problem, and when opening the last model in CBC. This is useful for checking the CBC arguments.</t>
   </si>
   <si>
-    <t>TODO:</t>
-  </si>
-  <si>
-    <t>Convert constants and formulae into the user's locale before displaying them in the Model dialog. OpenSolver currently converts new formulae from the users</t>
-  </si>
-  <si>
-    <t>locale into the internal US-locale on entry, but does not do the reverse on display. We need to put formulae into a cell, and read them back, to do this conversion.</t>
-  </si>
-  <si>
-    <t>1/</t>
-  </si>
-  <si>
     <t>Version 1.6 beta</t>
   </si>
   <si>
     <t>Fixed display and editting of an objective target value in the Model dialog.</t>
   </si>
   <si>
-    <t>As part of this, record in CConstraint a RHS either as a range, a value, or 'something else'. Then we can localise each of these more efficiently.</t>
-  </si>
-  <si>
     <t>Modified the Open Last Model in CBC functionality so that it passes any Solver options and any CBC solve parameters to CBC if they are available in any current worksheet</t>
   </si>
   <si>
@@ -360,15 +345,6 @@
   </si>
   <si>
     <t>Fixed a redim bug in the quick non-linearity checker for models with no constraints (which can happen if there is only a target objective value)</t>
-  </si>
-  <si>
-    <t>2/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pipe the CBC output so that it is visible to the user; see </t>
-  </si>
-  <si>
-    <t>http://www.vbforums.com/archive/index.php/t-47843.html</t>
   </si>
   <si>
     <t>Added "Show optimisation progress while solving"  (being Solver's "Show Iteration Results") to the OpenSolver options dialog</t>
@@ -643,6 +619,57 @@
   </si>
   <si>
     <t>Bugfixes for NEOS solvers</t>
+  </si>
+  <si>
+    <t>Add extra parameter support to Gurobi (see http://opensolver.org/using-opensolver/#gurobi-params)</t>
+  </si>
+  <si>
+    <t>Fix issues with sensitivity analysis and missing variables</t>
+  </si>
+  <si>
+    <t>Abort NEOS solve if Cancel button is clicked</t>
+  </si>
+  <si>
+    <t>Add better error message for when non-linear solvers create no solution file</t>
+  </si>
+  <si>
+    <t>Bonmin, Couenne and Gurobi support Solver Options (e.g. time limit, tolerance)</t>
+  </si>
+  <si>
+    <t>Support for running from multiple disks and network drives in OS X</t>
+  </si>
+  <si>
+    <t>Misc improvements in non-linear parsing.</t>
+  </si>
+  <si>
+    <t>Update solvers to CBC 2.9.0, Bonmin 1.8.0 and Couenne 0.5.1</t>
+  </si>
+  <si>
+    <t>Fix for misc OS X Yosemite issues</t>
+  </si>
+  <si>
+    <t>Make the model dialogue box resizable.</t>
+  </si>
+  <si>
+    <t>Better logging and 'Show Optimisation Progress' support. Now works on Mac</t>
+  </si>
+  <si>
+    <t>Expand check for `solver_rlx` to all new Excel versions.</t>
+  </si>
+  <si>
+    <t>Bugfixes for locale-based issues</t>
+  </si>
+  <si>
+    <t>Support for more formulae in non-linear solvers (e.g. SUMIF)</t>
+  </si>
+  <si>
+    <t>Implement proper sheet name escaping for the formula parser.</t>
+  </si>
+  <si>
+    <t>Better error message if NOMAD is missing</t>
+  </si>
+  <si>
+    <t>Version 2.6.1</t>
   </si>
 </sst>
 </file>
@@ -1022,1269 +1049,1338 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T227"/>
+  <dimension ref="A1:T239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>202</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42051</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="2"/>
+        <v>186</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>189</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="1">
-        <v>41920</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>191</v>
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
-        <v>190</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>192</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
-        <v>191</v>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>193</v>
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
-        <v>187</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>194</v>
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
-        <v>188</v>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>195</v>
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="4" t="s">
-        <v>192</v>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>196</v>
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
-        <v>189</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>197</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
-        <v>193</v>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>198</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>199</v>
+      </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>184</v>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>200</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
-        <v>185</v>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>201</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="1">
+        <v>41920</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="2"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>179</v>
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>180</v>
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="2"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="4" t="s">
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="2"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" s="1">
-        <v>41810</v>
-      </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>172</v>
       </c>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>173</v>
       </c>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="2"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="1">
-        <v>41324</v>
-      </c>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="1"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A45" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C45" s="1"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C46" s="1"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="1">
+        <v>41810</v>
+      </c>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C47" s="1"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>160</v>
+      </c>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A50" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C50" s="1"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>161</v>
+      </c>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" s="1"/>
+        <v>162</v>
+      </c>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C53" s="1"/>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A54" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C54" s="1"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="1">
+        <v>41324</v>
+      </c>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C55" s="1"/>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C56" s="1"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C57" s="1"/>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C58" s="1"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C59" s="1"/>
       <c r="H59" s="5"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A61" s="2" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C66" s="1"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A63" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A64" s="4"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A65" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C65" s="1">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A67" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A69" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C69" s="1">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C81" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A70" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A73" s="2"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A74" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C74" s="1">
-        <v>40963</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A76" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A79" s="2"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A80" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C80" s="1">
-        <v>40882</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>131</v>
-      </c>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>142</v>
-      </c>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
         <v>133</v>
       </c>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C86" s="1">
-        <v>40877</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>127</v>
       </c>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>129</v>
       </c>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A90" s="2"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A91" s="2" t="s">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C92" s="1">
+        <v>40882</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>123</v>
+      </c>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>124</v>
+      </c>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>125</v>
+      </c>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>119</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A92" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A99" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C99" s="1">
-        <v>40815</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A100" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A110" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A111" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A112" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A113" s="2"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A114" s="2" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C111" s="1">
+        <v>40815</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C126" s="1">
         <v>40764</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A116" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>96</v>
       </c>
-      <c r="B117" s="5"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A118" t="s">
+      <c r="B129" s="5"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A119" s="4"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A120" s="2" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C132" s="1">
         <v>40755</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A121" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A122" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B123" s="5" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B124" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A125" s="4"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A126" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A127" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A128" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A129" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A130" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A131" t="s">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A132" s="4"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A133" t="s">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A134" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B135" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A136" s="4"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A137" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A138" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B139" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B140" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B141" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B142" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B143" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B144" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A145" s="4"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A146" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A148" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A149" s="4"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A150" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="4"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A152" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A153" s="2"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A154" s="2" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C166" s="1">
         <v>40731</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A155" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>60</v>
       </c>
-      <c r="C155" s="1"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A156" s="4" t="s">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C156" s="1"/>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A157" s="4" t="s">
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="1"/>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A158" s="4" t="s">
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C158" s="1"/>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A160" s="2" t="s">
+      <c r="C170" s="1"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C160" s="1">
+      <c r="C172" s="1">
         <v>40610</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A161" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A163" s="2" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C175" s="1">
         <v>40606</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A164" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A165" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A166" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A167" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B168" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B169" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B170" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B171" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B172" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B173" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A174" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B175" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B176" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B177" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A178" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B179" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B180" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A181" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B182" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A183" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B184" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B185" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B186" t="s">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B187" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B188" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B189" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A190" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B191" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B192" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B193" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A194" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B195" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B196" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A197" t="s">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B198" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A199" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B200" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A201" t="s">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B202" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A203" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B204" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A206" s="2" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B218" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B207" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B208" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="B209" t="s">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A212" s="2" t="s">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C212" s="3">
+      <c r="C224" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A213" t="s">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A216" s="2" t="s">
+    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C216" s="3">
+      <c r="C228" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A217" s="6" t="s">
+    <row r="229" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B217" s="7"/>
-      <c r="C217" s="7"/>
-      <c r="D217" s="7"/>
-      <c r="E217" s="7"/>
-      <c r="F217" s="7"/>
-      <c r="G217" s="7"/>
-      <c r="H217" s="7"/>
-      <c r="I217" s="7"/>
-      <c r="J217" s="7"/>
-      <c r="K217" s="7"/>
-      <c r="L217" s="7"/>
-      <c r="M217" s="7"/>
-      <c r="N217" s="7"/>
-      <c r="O217" s="7"/>
-      <c r="P217" s="7"/>
-      <c r="Q217" s="7"/>
-      <c r="R217" s="7"/>
-      <c r="S217" s="7"/>
-      <c r="T217" s="7"/>
-    </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A219" s="2" t="s">
+      <c r="B229" s="7"/>
+      <c r="C229" s="7"/>
+      <c r="D229" s="7"/>
+      <c r="E229" s="7"/>
+      <c r="F229" s="7"/>
+      <c r="G229" s="7"/>
+      <c r="H229" s="7"/>
+      <c r="I229" s="7"/>
+      <c r="J229" s="7"/>
+      <c r="K229" s="7"/>
+      <c r="L229" s="7"/>
+      <c r="M229" s="7"/>
+      <c r="N229" s="7"/>
+      <c r="O229" s="7"/>
+      <c r="P229" s="7"/>
+      <c r="Q229" s="7"/>
+      <c r="R229" s="7"/>
+      <c r="S229" s="7"/>
+      <c r="T229" s="7"/>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C219" s="3">
+      <c r="C231" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A220" s="6" t="s">
+    <row r="232" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B220" s="6"/>
-      <c r="C220" s="6"/>
-      <c r="D220" s="6"/>
-      <c r="E220" s="6"/>
-      <c r="F220" s="6"/>
-      <c r="G220" s="6"/>
-      <c r="H220" s="6"/>
-      <c r="I220" s="6"/>
-      <c r="J220" s="6"/>
-      <c r="K220" s="6"/>
-      <c r="L220" s="6"/>
-      <c r="M220" s="6"/>
-      <c r="N220" s="6"/>
-      <c r="O220" s="6"/>
-      <c r="P220" s="6"/>
-      <c r="Q220" s="6"/>
-      <c r="R220" s="6"/>
-      <c r="S220" s="6"/>
-      <c r="T220" s="6"/>
-    </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A222" s="2" t="s">
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+      <c r="D232" s="6"/>
+      <c r="E232" s="6"/>
+      <c r="F232" s="6"/>
+      <c r="G232" s="6"/>
+      <c r="H232" s="6"/>
+      <c r="I232" s="6"/>
+      <c r="J232" s="6"/>
+      <c r="K232" s="6"/>
+      <c r="L232" s="6"/>
+      <c r="M232" s="6"/>
+      <c r="N232" s="6"/>
+      <c r="O232" s="6"/>
+      <c r="P232" s="6"/>
+      <c r="Q232" s="6"/>
+      <c r="R232" s="6"/>
+      <c r="S232" s="6"/>
+      <c r="T232" s="6"/>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C222" s="3">
+      <c r="C234" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A223" s="6" t="s">
+    <row r="235" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B223" s="6"/>
-      <c r="C223" s="6"/>
-      <c r="D223" s="6"/>
-      <c r="E223" s="6"/>
-      <c r="F223" s="6"/>
-      <c r="G223" s="6"/>
-      <c r="H223" s="6"/>
-      <c r="I223" s="6"/>
-      <c r="J223" s="6"/>
-      <c r="K223" s="6"/>
-      <c r="L223" s="6"/>
-      <c r="M223" s="6"/>
-      <c r="N223" s="6"/>
-      <c r="O223" s="6"/>
-      <c r="P223" s="6"/>
-      <c r="Q223" s="6"/>
-      <c r="R223" s="6"/>
-      <c r="S223" s="6"/>
-      <c r="T223" s="6"/>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A226" s="2" t="s">
+      <c r="B235" s="6"/>
+      <c r="C235" s="6"/>
+      <c r="D235" s="6"/>
+      <c r="E235" s="6"/>
+      <c r="F235" s="6"/>
+      <c r="G235" s="6"/>
+      <c r="H235" s="6"/>
+      <c r="I235" s="6"/>
+      <c r="J235" s="6"/>
+      <c r="K235" s="6"/>
+      <c r="L235" s="6"/>
+      <c r="M235" s="6"/>
+      <c r="N235" s="6"/>
+      <c r="O235" s="6"/>
+      <c r="P235" s="6"/>
+      <c r="Q235" s="6"/>
+      <c r="R235" s="6"/>
+      <c r="S235" s="6"/>
+      <c r="T235" s="6"/>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C226" s="3">
+      <c r="C238" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A227" t="s">
+    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A217:T217"/>
-    <mergeCell ref="A220:T220"/>
-    <mergeCell ref="A223:T223"/>
+    <mergeCell ref="A229:T229"/>
+    <mergeCell ref="A232:T232"/>
+    <mergeCell ref="A235:T235"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B123" r:id="rId1"/>
-    <hyperlink ref="H7" r:id="rId2"/>
+    <hyperlink ref="B135" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2295,7 +2391,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2308,7 +2404,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update changelog for release
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$127</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$136</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="211">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -670,6 +670,30 @@
   </si>
   <si>
     <t>Version 2.6.1</t>
+  </si>
+  <si>
+    <t>Add Update Checker</t>
+  </si>
+  <si>
+    <t>Add OpenSolver API VBA interface</t>
+  </si>
+  <si>
+    <t>Revamped error reporting with email reports</t>
+  </si>
+  <si>
+    <t>All solvers support extra parameters</t>
+  </si>
+  <si>
+    <t>Experimental support for NOMAD on Mac</t>
+  </si>
+  <si>
+    <t>Update solvers to CBC 2.9.4, Bonmin 1.8.1, Couenne 0.5.3, NOMAD 3.7.2</t>
+  </si>
+  <si>
+    <t>Various bugfixes (including lots of locale issues)</t>
+  </si>
+  <si>
+    <t>Version 2.7.0</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1073,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T239"/>
+  <dimension ref="A1:T248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,161 +1095,161 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42171</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C12" s="1">
         <v>42051</v>
-      </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>186</v>
-      </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>187</v>
-      </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>188</v>
-      </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>189</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>191</v>
-      </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>192</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>193</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>194</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>193</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>196</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>200</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>201</v>
-      </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="1">
-        <v>41920</v>
-      </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="H28" s="5"/>
     </row>
@@ -1235,697 +1259,709 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
+      </c>
+      <c r="C30" s="1">
+        <v>41920</v>
       </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>174</v>
+      <c r="A33" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="A35" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>171</v>
+      <c r="A36" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>173</v>
-      </c>
+      <c r="A38" s="2"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>166</v>
+      <c r="A40" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>167</v>
-      </c>
+      <c r="A41" s="2"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>170</v>
+      <c r="A42" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>169</v>
-      </c>
+      <c r="A44" s="2"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" s="1">
-        <v>41810</v>
+      <c r="A46" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" s="1"/>
+        <v>173</v>
+      </c>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>160</v>
-      </c>
+      <c r="A48" s="2"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>164</v>
+      <c r="A49" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+      <c r="A53" s="4" t="s">
+        <v>169</v>
+      </c>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C54" s="1">
-        <v>41324</v>
-      </c>
+      <c r="A54" s="2"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C55" s="1"/>
+      <c r="A55" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C55" s="1">
+        <v>41810</v>
+      </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C56" s="1"/>
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="1"/>
+        <v>160</v>
+      </c>
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C58" s="1"/>
+        <v>164</v>
+      </c>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C59" s="1"/>
+        <v>165</v>
+      </c>
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C60" s="1"/>
+        <v>161</v>
+      </c>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C61" s="1"/>
+        <v>162</v>
+      </c>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C62" s="1"/>
+      <c r="A62" s="2"/>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C63" s="1"/>
+      <c r="A63" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="1">
+        <v>41324</v>
+      </c>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C64" s="1"/>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C65" s="1"/>
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C66" s="1"/>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C67" s="1"/>
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C68" s="1"/>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C69" s="1"/>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C70" s="1"/>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C71" s="1"/>
       <c r="H71" s="5"/>
     </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="H72" s="5"/>
+    </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C73" s="1">
-        <v>41211</v>
-      </c>
+      <c r="A73" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>140</v>
-      </c>
+      <c r="A74" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>139</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
+      <c r="A76" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C77" s="1">
-        <v>41176</v>
-      </c>
+      <c r="A77" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>136</v>
-      </c>
+      <c r="A78" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>137</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C81" s="1">
-        <v>41157</v>
-      </c>
+      <c r="A80" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="H80" s="5"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>132</v>
+      <c r="A82" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" s="1">
+        <v>41211</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>133</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
+      <c r="A85" s="4"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C86" s="1">
-        <v>40963</v>
+        <v>41176</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>129</v>
-      </c>
+      <c r="A89" s="2"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>130</v>
+      <c r="A90" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C90" s="1">
+        <v>41157</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
+      <c r="A91" s="4" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C92" s="1">
-        <v>40882</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>123</v>
-      </c>
-      <c r="C93" s="1"/>
+      <c r="A92" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>124</v>
-      </c>
-      <c r="C94" s="1"/>
+      <c r="A94" s="2"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>134</v>
-      </c>
-      <c r="C95" s="1"/>
+      <c r="A95" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C95" s="1">
+        <v>40963</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>125</v>
-      </c>
-      <c r="C96" s="1"/>
+        <v>127</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
+      <c r="A97" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C98" s="1">
-        <v>40877</v>
+      <c r="A98" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>119</v>
-      </c>
-      <c r="C99" s="1"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C100" s="1"/>
+      <c r="A100" s="2"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>120</v>
+      <c r="A101" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="1">
+        <v>40882</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
+      <c r="A102" t="s">
+        <v>123</v>
+      </c>
+      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C103" s="1">
-        <v>40858</v>
-      </c>
+      <c r="A103" t="s">
+        <v>124</v>
+      </c>
+      <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>117</v>
+      <c r="A104" t="s">
+        <v>134</v>
       </c>
       <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>112</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C105" s="1"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>113</v>
-      </c>
+      <c r="A106" s="2"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>115</v>
+      <c r="A107" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C107" s="1">
+        <v>40877</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>114</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>116</v>
-      </c>
+      <c r="A109" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="2"/>
+      <c r="A110" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C111" s="1">
-        <v>40815</v>
-      </c>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>98</v>
+      <c r="A112" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C112" s="1">
+        <v>40858</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>99</v>
-      </c>
+      <c r="A113" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>105</v>
-      </c>
+      <c r="A119" s="2"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>106</v>
+      <c r="A120" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C120" s="1">
+        <v>40815</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>107</v>
+      <c r="A121" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="2"/>
+      <c r="A125" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C126" s="1">
-        <v>40764</v>
+      <c r="A126" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>96</v>
-      </c>
-      <c r="B129" s="5"/>
+        <v>106</v>
+      </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="4"/>
+      <c r="A131" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C132" s="1">
-        <v>40755</v>
+      <c r="A132" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>66</v>
-      </c>
+      <c r="A134" s="2"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="5" t="s">
-        <v>64</v>
+      <c r="A135" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" s="1">
+        <v>40764</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>67</v>
+      <c r="A136" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="4"/>
+      <c r="A137" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>68</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B138" s="5"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>70</v>
-      </c>
+      <c r="A140" s="4"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>71</v>
+      <c r="A141" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C141" s="1">
+        <v>40755</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="4"/>
+      <c r="B144" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>74</v>
+      <c r="B145" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>75</v>
-      </c>
+      <c r="A146" s="4"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B147" t="s">
-        <v>76</v>
+      <c r="A147" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="4"/>
+      <c r="A148" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B151" t="s">
-        <v>79</v>
+      <c r="A151" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
-        <v>80</v>
+      <c r="A152" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B153" t="s">
-        <v>81</v>
-      </c>
+      <c r="A153" s="4"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>82</v>
+      <c r="A154" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B155" t="s">
-        <v>83</v>
+      <c r="A155" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -1933,451 +1969,494 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>87</v>
+      <c r="B160" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="4"/>
+      <c r="B161" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>88</v>
+      <c r="B162" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>89</v>
+      <c r="B163" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>90</v>
+      <c r="B164" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="2"/>
+      <c r="B165" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C166" s="1">
-        <v>40731</v>
-      </c>
+      <c r="A166" s="4"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>60</v>
-      </c>
-      <c r="C167" s="1"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C168" s="1"/>
+      <c r="A168" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C169" s="1"/>
+      <c r="A169" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C170" s="1"/>
+      <c r="A170" s="4"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C172" s="1">
-        <v>40610</v>
+      <c r="A172" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>58</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C175" s="1">
-        <v>40606</v>
+        <v>40731</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>60</v>
+      </c>
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C179" s="1"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C181" s="1">
+        <v>40610</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C184" s="1">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B191" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>36</v>
+      <c r="A199" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>30</v>
+      <c r="A204" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>25</v>
+      <c r="B206" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
+    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B227" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
+    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
+    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
+    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
+    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C224" s="3">
+      <c r="C233" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
+    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C228" s="3">
+      <c r="C237" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="6" t="s">
+    <row r="238" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B229" s="7"/>
-      <c r="C229" s="7"/>
-      <c r="D229" s="7"/>
-      <c r="E229" s="7"/>
-      <c r="F229" s="7"/>
-      <c r="G229" s="7"/>
-      <c r="H229" s="7"/>
-      <c r="I229" s="7"/>
-      <c r="J229" s="7"/>
-      <c r="K229" s="7"/>
-      <c r="L229" s="7"/>
-      <c r="M229" s="7"/>
-      <c r="N229" s="7"/>
-      <c r="O229" s="7"/>
-      <c r="P229" s="7"/>
-      <c r="Q229" s="7"/>
-      <c r="R229" s="7"/>
-      <c r="S229" s="7"/>
-      <c r="T229" s="7"/>
-    </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
+      <c r="B238" s="7"/>
+      <c r="C238" s="7"/>
+      <c r="D238" s="7"/>
+      <c r="E238" s="7"/>
+      <c r="F238" s="7"/>
+      <c r="G238" s="7"/>
+      <c r="H238" s="7"/>
+      <c r="I238" s="7"/>
+      <c r="J238" s="7"/>
+      <c r="K238" s="7"/>
+      <c r="L238" s="7"/>
+      <c r="M238" s="7"/>
+      <c r="N238" s="7"/>
+      <c r="O238" s="7"/>
+      <c r="P238" s="7"/>
+      <c r="Q238" s="7"/>
+      <c r="R238" s="7"/>
+      <c r="S238" s="7"/>
+      <c r="T238" s="7"/>
+    </row>
+    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C231" s="3">
+      <c r="C240" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="6" t="s">
+    <row r="241" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B232" s="6"/>
-      <c r="C232" s="6"/>
-      <c r="D232" s="6"/>
-      <c r="E232" s="6"/>
-      <c r="F232" s="6"/>
-      <c r="G232" s="6"/>
-      <c r="H232" s="6"/>
-      <c r="I232" s="6"/>
-      <c r="J232" s="6"/>
-      <c r="K232" s="6"/>
-      <c r="L232" s="6"/>
-      <c r="M232" s="6"/>
-      <c r="N232" s="6"/>
-      <c r="O232" s="6"/>
-      <c r="P232" s="6"/>
-      <c r="Q232" s="6"/>
-      <c r="R232" s="6"/>
-      <c r="S232" s="6"/>
-      <c r="T232" s="6"/>
-    </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A234" s="2" t="s">
+      <c r="B241" s="6"/>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
+      <c r="E241" s="6"/>
+      <c r="F241" s="6"/>
+      <c r="G241" s="6"/>
+      <c r="H241" s="6"/>
+      <c r="I241" s="6"/>
+      <c r="J241" s="6"/>
+      <c r="K241" s="6"/>
+      <c r="L241" s="6"/>
+      <c r="M241" s="6"/>
+      <c r="N241" s="6"/>
+      <c r="O241" s="6"/>
+      <c r="P241" s="6"/>
+      <c r="Q241" s="6"/>
+      <c r="R241" s="6"/>
+      <c r="S241" s="6"/>
+      <c r="T241" s="6"/>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C234" s="3">
+      <c r="C243" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="6" t="s">
+    <row r="244" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B235" s="6"/>
-      <c r="C235" s="6"/>
-      <c r="D235" s="6"/>
-      <c r="E235" s="6"/>
-      <c r="F235" s="6"/>
-      <c r="G235" s="6"/>
-      <c r="H235" s="6"/>
-      <c r="I235" s="6"/>
-      <c r="J235" s="6"/>
-      <c r="K235" s="6"/>
-      <c r="L235" s="6"/>
-      <c r="M235" s="6"/>
-      <c r="N235" s="6"/>
-      <c r="O235" s="6"/>
-      <c r="P235" s="6"/>
-      <c r="Q235" s="6"/>
-      <c r="R235" s="6"/>
-      <c r="S235" s="6"/>
-      <c r="T235" s="6"/>
-    </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A238" s="2" t="s">
+      <c r="B244" s="6"/>
+      <c r="C244" s="6"/>
+      <c r="D244" s="6"/>
+      <c r="E244" s="6"/>
+      <c r="F244" s="6"/>
+      <c r="G244" s="6"/>
+      <c r="H244" s="6"/>
+      <c r="I244" s="6"/>
+      <c r="J244" s="6"/>
+      <c r="K244" s="6"/>
+      <c r="L244" s="6"/>
+      <c r="M244" s="6"/>
+      <c r="N244" s="6"/>
+      <c r="O244" s="6"/>
+      <c r="P244" s="6"/>
+      <c r="Q244" s="6"/>
+      <c r="R244" s="6"/>
+      <c r="S244" s="6"/>
+      <c r="T244" s="6"/>
+    </row>
+    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C238" s="3">
+      <c r="C247" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
+    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A229:T229"/>
-    <mergeCell ref="A232:T232"/>
-    <mergeCell ref="A235:T235"/>
+    <mergeCell ref="A238:T238"/>
+    <mergeCell ref="A241:T241"/>
+    <mergeCell ref="A244:T244"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B135" r:id="rId1"/>
+    <hyperlink ref="B144" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Bump version for release
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$136</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$139</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="213">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -694,6 +694,12 @@
   </si>
   <si>
     <t>Version 2.7.0</t>
+  </si>
+  <si>
+    <t>Version 2.7.1</t>
+  </si>
+  <si>
+    <t>Various bugfixes for 2.7.0</t>
   </si>
 </sst>
 </file>
@@ -1073,10 +1079,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T248"/>
+  <dimension ref="A1:T251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,232 +1101,235 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C3" s="1">
-        <v>42171</v>
+        <v>42183</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>204</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>205</v>
+      <c r="A6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42171</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="1">
         <v>42051</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>186</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>187</v>
-      </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>188</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>199</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>200</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>201</v>
       </c>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C33" s="1">
         <v>41920</v>
-      </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+      <c r="A38" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>176</v>
+      <c r="A39" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H40" s="5"/>
     </row>
@@ -1330,13 +1339,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H43" s="5"/>
     </row>
@@ -1346,1063 +1355,1047 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>170</v>
-      </c>
+      <c r="A51" s="2"/>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>168</v>
+      <c r="A52" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
+      <c r="A54" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="1">
-        <v>41810</v>
+      <c r="A55" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" s="1"/>
+        <v>169</v>
+      </c>
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>160</v>
-      </c>
+      <c r="A57" s="2"/>
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>164</v>
+      <c r="A58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="1">
+        <v>41810</v>
       </c>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>165</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C59" s="1"/>
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
+      <c r="A62" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C63" s="1">
-        <v>41324</v>
+      <c r="A63" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C64" s="1"/>
+        <v>162</v>
+      </c>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C65" s="1"/>
+      <c r="A65" s="2"/>
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C66" s="1"/>
+      <c r="A66" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="1">
+        <v>41324</v>
+      </c>
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C67" s="1"/>
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C68" s="1"/>
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C69" s="1"/>
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C70" s="1"/>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C71" s="1"/>
       <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C72" s="1"/>
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C73" s="1"/>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C74" s="1"/>
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C75" s="1"/>
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C76" s="1"/>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C77" s="1"/>
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C78" s="1"/>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="1"/>
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C80" s="1"/>
       <c r="H80" s="5"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C85" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C89" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C93" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C98" s="1">
         <v>40963</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
+      <c r="A100" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C101" s="1">
-        <v>40882</v>
+      <c r="A101" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>123</v>
-      </c>
-      <c r="C102" s="1"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>124</v>
-      </c>
-      <c r="C103" s="1"/>
+      <c r="A103" s="2"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>134</v>
-      </c>
-      <c r="C104" s="1"/>
+      <c r="A104" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="1">
+        <v>40882</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C105" s="1"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
+      <c r="A106" t="s">
+        <v>124</v>
+      </c>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C107" s="1">
-        <v>40877</v>
-      </c>
+      <c r="A107" t="s">
+        <v>134</v>
+      </c>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>125</v>
+      </c>
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>119</v>
       </c>
-      <c r="C108" s="1"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C109" s="1"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C115" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C113" s="1"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>115</v>
-      </c>
+      <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C123" s="1">
         <v>40815</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="2"/>
+      <c r="A134" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C135" s="1">
-        <v>40764</v>
+      <c r="A135" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>94</v>
-      </c>
+      <c r="A137" s="2"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>96</v>
-      </c>
-      <c r="B138" s="5"/>
+      <c r="A138" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C138" s="1">
+        <v>40764</v>
+      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="4"/>
+      <c r="A140" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C141" s="1">
-        <v>40755</v>
-      </c>
+      <c r="A141" t="s">
+        <v>96</v>
+      </c>
+      <c r="B141" s="5"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C144" s="1">
+        <v>40755</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="5" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="4"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>70</v>
-      </c>
+      <c r="A149" s="4"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="4"/>
+      <c r="A153" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
-        <v>76</v>
-      </c>
+      <c r="A156" s="4"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="4"/>
+      <c r="A157" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="4"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="4"/>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="4"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="4"/>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="4"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="2"/>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="2"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C175" s="1">
+      <c r="C178" s="1">
         <v>40731</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>60</v>
       </c>
-      <c r="C176" s="1"/>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="4" t="s">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C177" s="1"/>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="4" t="s">
+      <c r="C180" s="1"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C178" s="1"/>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="4" t="s">
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C179" s="1"/>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C181" s="1">
-        <v>40610</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>58</v>
-      </c>
+      <c r="C182" s="1"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C184" s="1">
-        <v>40606</v>
+        <v>40610</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>3</v>
+      <c r="A187" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C187" s="1">
+        <v>40606</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B191" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>10</v>
+      <c r="B195" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>24</v>
+      <c r="A198" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>13</v>
+      <c r="B199" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>19</v>
+      <c r="B204" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B205" t="s">
-        <v>18</v>
+      <c r="A205" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
-        <v>29</v>
+      <c r="A207" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>22</v>
+      <c r="B211" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>31</v>
+      <c r="A214" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>25</v>
+      <c r="B215" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B225" t="s">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B230" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B230" t="s">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C233" s="3">
+      <c r="C236" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C237" s="3">
+      <c r="C240" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="6" t="s">
+    <row r="241" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B238" s="7"/>
-      <c r="C238" s="7"/>
-      <c r="D238" s="7"/>
-      <c r="E238" s="7"/>
-      <c r="F238" s="7"/>
-      <c r="G238" s="7"/>
-      <c r="H238" s="7"/>
-      <c r="I238" s="7"/>
-      <c r="J238" s="7"/>
-      <c r="K238" s="7"/>
-      <c r="L238" s="7"/>
-      <c r="M238" s="7"/>
-      <c r="N238" s="7"/>
-      <c r="O238" s="7"/>
-      <c r="P238" s="7"/>
-      <c r="Q238" s="7"/>
-      <c r="R238" s="7"/>
-      <c r="S238" s="7"/>
-      <c r="T238" s="7"/>
-    </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C240" s="3">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="241" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B241" s="6"/>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="G241" s="6"/>
-      <c r="H241" s="6"/>
-      <c r="I241" s="6"/>
-      <c r="J241" s="6"/>
-      <c r="K241" s="6"/>
-      <c r="L241" s="6"/>
-      <c r="M241" s="6"/>
-      <c r="N241" s="6"/>
-      <c r="O241" s="6"/>
-      <c r="P241" s="6"/>
-      <c r="Q241" s="6"/>
-      <c r="R241" s="6"/>
-      <c r="S241" s="6"/>
-      <c r="T241" s="6"/>
+      <c r="B241" s="7"/>
+      <c r="C241" s="7"/>
+      <c r="D241" s="7"/>
+      <c r="E241" s="7"/>
+      <c r="F241" s="7"/>
+      <c r="G241" s="7"/>
+      <c r="H241" s="7"/>
+      <c r="I241" s="7"/>
+      <c r="J241" s="7"/>
+      <c r="K241" s="7"/>
+      <c r="L241" s="7"/>
+      <c r="M241" s="7"/>
+      <c r="N241" s="7"/>
+      <c r="O241" s="7"/>
+      <c r="P241" s="7"/>
+      <c r="Q241" s="7"/>
+      <c r="R241" s="7"/>
+      <c r="S241" s="7"/>
+      <c r="T241" s="7"/>
     </row>
     <row r="243" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
@@ -2414,7 +2407,7 @@
     </row>
     <row r="244" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
@@ -2436,27 +2429,59 @@
       <c r="S244" s="6"/>
       <c r="T244" s="6"/>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
+    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C246" s="3">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="247" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B247" s="6"/>
+      <c r="C247" s="6"/>
+      <c r="D247" s="6"/>
+      <c r="E247" s="6"/>
+      <c r="F247" s="6"/>
+      <c r="G247" s="6"/>
+      <c r="H247" s="6"/>
+      <c r="I247" s="6"/>
+      <c r="J247" s="6"/>
+      <c r="K247" s="6"/>
+      <c r="L247" s="6"/>
+      <c r="M247" s="6"/>
+      <c r="N247" s="6"/>
+      <c r="O247" s="6"/>
+      <c r="P247" s="6"/>
+      <c r="Q247" s="6"/>
+      <c r="R247" s="6"/>
+      <c r="S247" s="6"/>
+      <c r="T247" s="6"/>
+    </row>
+    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C247" s="3">
+      <c r="C250" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
+    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A238:T238"/>
     <mergeCell ref="A241:T241"/>
     <mergeCell ref="A244:T244"/>
+    <mergeCell ref="A247:T247"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B144" r:id="rId1"/>
+    <hyperlink ref="B147" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Update changelog for 2.8.0
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26709"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Dropbox (Personal)\Scratch\OpenSolver\OpenSolver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Dropbox (Personal)/Scratch/OpenSolver/OpenSolver/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="13905"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$139</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$187</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -34,12 +34,17 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="260">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -700,6 +705,147 @@
   </si>
   <si>
     <t>Various bugfixes for 2.7.0</t>
+  </si>
+  <si>
+    <t>Changes to modeling</t>
+  </si>
+  <si>
+    <t>- Ranges don't have to be on the model sheet</t>
+  </si>
+  <si>
+    <t>Console form now shows optimisation progress including streaming output from solver and easy cancel</t>
+  </si>
+  <si>
+    <t>New menu items</t>
+  </si>
+  <si>
+    <t>Changes to API</t>
+  </si>
+  <si>
+    <t>- GetObjectiveFunctionCell validate parameter defaults to True</t>
+  </si>
+  <si>
+    <t>Miscellaneous bugfixes/improvements</t>
+  </si>
+  <si>
+    <t>- Improved reading of .sol file for NL solvers</t>
+  </si>
+  <si>
+    <t>- Improvements to Gurobi solution reader (c/o Greg Glockner at Gurobi) for better cloud support</t>
+  </si>
+  <si>
+    <t>- Model form doesn't delete missing references on load</t>
+  </si>
+  <si>
+    <t>Version 2.8.0</t>
+  </si>
+  <si>
+    <t>- Can use named ranges to define the model</t>
+  </si>
+  <si>
+    <t>Support for PRODUCT function in nonlinear solvers</t>
+  </si>
+  <si>
+    <t>- View error log file</t>
+  </si>
+  <si>
+    <t>- View all OpenSolver temp files</t>
+  </si>
+  <si>
+    <t>"About OpenSolver" form includes a check for whether OpenSolver is installed correctly</t>
+  </si>
+  <si>
+    <t>- Deleted GetObjectiveFunctionCellWithValidation</t>
+  </si>
+  <si>
+    <t>- Addition of RefersTo methods for working with named ranges (and optional RefersTo return parameters in Get methods)</t>
+  </si>
+  <si>
+    <t>- API methods now validate the inputs and outputs</t>
+  </si>
+  <si>
+    <t>- Fix duplicate key error when loading model form</t>
+  </si>
+  <si>
+    <t>- Only load an NL solution if the solver returns solution</t>
+  </si>
+  <si>
+    <t>- Fix for Mac form bug on Yosemite</t>
+  </si>
+  <si>
+    <t>- NL writing to file is buffered</t>
+  </si>
+  <si>
+    <t>- Fix errors when setting QuickSolve parameters range</t>
+  </si>
+  <si>
+    <t>- temp files live in a subfolder and are cleaned up when Excel exits</t>
+  </si>
+  <si>
+    <t>- Revamped menu layout, generated programmatically for Windows and Mac</t>
+  </si>
+  <si>
+    <t>- New backend for running external commands, Improvements for piping and termination</t>
+  </si>
+  <si>
+    <t>- Fix headings on sensitivity report</t>
+  </si>
+  <si>
+    <t>- Add suggestion to restart Excel when log file is locked</t>
+  </si>
+  <si>
+    <t>- Make ConvertLocale a no-op if already in US locale</t>
+  </si>
+  <si>
+    <t>- Only use numeric RHS values as bounds</t>
+  </si>
+  <si>
+    <t>- Fix overflow error in CBC solution reader</t>
+  </si>
+  <si>
+    <t>- Fix variable count in status bar while solving</t>
+  </si>
+  <si>
+    <t>- Fix localisation error in update checker</t>
+  </si>
+  <si>
+    <t>- Better escape handling in all solvers</t>
+  </si>
+  <si>
+    <t>- Fix garbage in error reports on Mac</t>
+  </si>
+  <si>
+    <t>- Fix ordering of variables in LP file to Make sensitivity table correct</t>
+  </si>
+  <si>
+    <t>- New default for linearity check, and Better detection of non-linearity, including before solve</t>
+  </si>
+  <si>
+    <t>- Fix focus issue with error dialog</t>
+  </si>
+  <si>
+    <t>- Raise error on non-numeric constants in parser</t>
+  </si>
+  <si>
+    <t>- Refactor COpenSolver to remove redundant code and Better separate difference model into CModelDiff</t>
+  </si>
+  <si>
+    <t>- Raise error when sheet has been Deleted in reference</t>
+  </si>
+  <si>
+    <t>- Fix /amplin error on NEOS</t>
+  </si>
+  <si>
+    <t>- Increase time between NEOS checks to support changes made by NEOS server-side</t>
+  </si>
+  <si>
+    <t>- Fix RefEdit focus bugs on model form</t>
+  </si>
+  <si>
+    <t>- backend changes to model form to handle named ranges as model parameters</t>
+  </si>
+  <si>
+    <t>- Tidyup of names storage backend</t>
   </si>
 </sst>
 </file>
@@ -760,7 +906,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -773,6 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -837,9 +984,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -872,9 +1019,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1078,1410 +1225,1697 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T251"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:T299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C51" s="1">
         <v>42183</v>
       </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C54" s="1">
         <v>42171</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C63" s="1">
         <v>42051</v>
       </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>186</v>
       </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>187</v>
       </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>188</v>
       </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>189</v>
       </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>190</v>
       </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>191</v>
       </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>192</v>
       </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>193</v>
       </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>194</v>
       </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>195</v>
       </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>196</v>
       </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>197</v>
       </c>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>198</v>
       </c>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>199</v>
       </c>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>200</v>
       </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>201</v>
       </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C81" s="1">
         <v>41920</v>
       </c>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="2"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="2"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="2"/>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="2"/>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="H104" s="5"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="2"/>
+      <c r="H105" s="5"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C106" s="1">
         <v>41810</v>
       </c>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="H106" s="5"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="C107" s="1"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="H108" s="5"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="H109" s="5"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="H62" s="5"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="H110" s="5"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="H63" s="5"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="H111" s="5"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="H112" s="5"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="2"/>
+      <c r="H113" s="5"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C114" s="1">
         <v>41324</v>
       </c>
-      <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="H114" s="5"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="1"/>
-      <c r="H67" s="5"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="C115" s="1"/>
+      <c r="H115" s="5"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C68" s="1"/>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="C116" s="1"/>
+      <c r="H116" s="5"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="C117" s="1"/>
+      <c r="H117" s="5"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="1"/>
-      <c r="H70" s="5"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="C118" s="1"/>
+      <c r="H118" s="5"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="H71" s="5"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="C119" s="1"/>
+      <c r="H119" s="5"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C72" s="1"/>
-      <c r="H72" s="5"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="C120" s="1"/>
+      <c r="H120" s="5"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C73" s="1"/>
-      <c r="H73" s="5"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="C121" s="1"/>
+      <c r="H121" s="5"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C74" s="1"/>
-      <c r="H74" s="5"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="C122" s="1"/>
+      <c r="H122" s="5"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="1"/>
-      <c r="H75" s="5"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="C123" s="1"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C76" s="1"/>
-      <c r="H76" s="5"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="C124" s="1"/>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C77" s="1"/>
-      <c r="H77" s="5"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="C125" s="1"/>
+      <c r="H125" s="5"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="1"/>
-      <c r="H78" s="5"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="C126" s="1"/>
+      <c r="H126" s="5"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C79" s="1"/>
-      <c r="H79" s="5"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="C127" s="1"/>
+      <c r="H127" s="5"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C80" s="1"/>
-      <c r="H80" s="5"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="C128" s="1"/>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="H81" s="5"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="C129" s="1"/>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C82" s="1"/>
-      <c r="H82" s="5"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+      <c r="C130" s="1"/>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C83" s="1"/>
-      <c r="H83" s="5"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="C131" s="1"/>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C133" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" s="4"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C137" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="2"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C141" s="1">
         <v>41157</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="2"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C146" s="1">
         <v>40963</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="2"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C152" s="1">
         <v>40882</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>123</v>
       </c>
-      <c r="C105" s="1"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="C153" s="1"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>124</v>
       </c>
-      <c r="C106" s="1"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>134</v>
       </c>
-      <c r="C107" s="1"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>125</v>
       </c>
-      <c r="C108" s="1"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="2"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C110" s="1">
+      <c r="C158" s="1">
         <v>40877</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>119</v>
       </c>
-      <c r="C111" s="1"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C112" s="1"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="2"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="2"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C163" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C116" s="1"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="2"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="2"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C123" s="1">
+      <c r="C171" s="1">
         <v>40815</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="2"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="2"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C186" s="1">
         <v>40764</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
         <v>96</v>
       </c>
-      <c r="B141" s="5"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="B189" s="5"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="4"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="4"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C192" s="1">
         <v>40755</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="5" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B195" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="4"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="4"/>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="4"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="4"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B207" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="4"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="4"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B211" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B212" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B213" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B214" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B215" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B216" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="4"/>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="4"/>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="4"/>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="4"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="2"/>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="2" t="s">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="2"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C178" s="1">
+      <c r="C226" s="1">
         <v>40731</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
         <v>60</v>
       </c>
-      <c r="C179" s="1"/>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="4" t="s">
+      <c r="C227" s="1"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C180" s="1"/>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="4" t="s">
+      <c r="C228" s="1"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C181" s="1"/>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="4" t="s">
+      <c r="C229" s="1"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C182" s="1"/>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+      <c r="C230" s="1"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C184" s="1">
+      <c r="C232" s="1">
         <v>40610</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C187" s="1">
+      <c r="C235" s="1">
         <v>40606</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B240" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B241" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B242" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B243" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B244" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B245" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B247" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B248" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B249" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B251" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B252" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B254" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B256" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B257" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B258" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B259" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B260" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B261" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B215" t="s">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B263" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B264" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B265" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B267" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B268" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B222" t="s">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B270" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B272" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B274" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B276" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B278" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B231" t="s">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B279" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B232" t="s">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B280" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B233" t="s">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B281" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C236" s="3">
+      <c r="C284" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C240" s="3">
+      <c r="C288" s="3">
         <v>40375</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="6" t="s">
+    <row r="289" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B241" s="7"/>
-      <c r="C241" s="7"/>
-      <c r="D241" s="7"/>
-      <c r="E241" s="7"/>
-      <c r="F241" s="7"/>
-      <c r="G241" s="7"/>
-      <c r="H241" s="7"/>
-      <c r="I241" s="7"/>
-      <c r="J241" s="7"/>
-      <c r="K241" s="7"/>
-      <c r="L241" s="7"/>
-      <c r="M241" s="7"/>
-      <c r="N241" s="7"/>
-      <c r="O241" s="7"/>
-      <c r="P241" s="7"/>
-      <c r="Q241" s="7"/>
-      <c r="R241" s="7"/>
-      <c r="S241" s="7"/>
-      <c r="T241" s="7"/>
-    </row>
-    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
+      <c r="B289" s="7"/>
+      <c r="C289" s="7"/>
+      <c r="D289" s="7"/>
+      <c r="E289" s="7"/>
+      <c r="F289" s="7"/>
+      <c r="G289" s="7"/>
+      <c r="H289" s="7"/>
+      <c r="I289" s="7"/>
+      <c r="J289" s="7"/>
+      <c r="K289" s="7"/>
+      <c r="L289" s="7"/>
+      <c r="M289" s="7"/>
+      <c r="N289" s="7"/>
+      <c r="O289" s="7"/>
+      <c r="P289" s="7"/>
+      <c r="Q289" s="7"/>
+      <c r="R289" s="7"/>
+      <c r="S289" s="7"/>
+      <c r="T289" s="7"/>
+    </row>
+    <row r="291" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A291" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C243" s="3">
+      <c r="C291" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="6" t="s">
+    <row r="292" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B244" s="6"/>
-      <c r="C244" s="6"/>
-      <c r="D244" s="6"/>
-      <c r="E244" s="6"/>
-      <c r="F244" s="6"/>
-      <c r="G244" s="6"/>
-      <c r="H244" s="6"/>
-      <c r="I244" s="6"/>
-      <c r="J244" s="6"/>
-      <c r="K244" s="6"/>
-      <c r="L244" s="6"/>
-      <c r="M244" s="6"/>
-      <c r="N244" s="6"/>
-      <c r="O244" s="6"/>
-      <c r="P244" s="6"/>
-      <c r="Q244" s="6"/>
-      <c r="R244" s="6"/>
-      <c r="S244" s="6"/>
-      <c r="T244" s="6"/>
-    </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
+      <c r="B292" s="6"/>
+      <c r="C292" s="6"/>
+      <c r="D292" s="6"/>
+      <c r="E292" s="6"/>
+      <c r="F292" s="6"/>
+      <c r="G292" s="6"/>
+      <c r="H292" s="6"/>
+      <c r="I292" s="6"/>
+      <c r="J292" s="6"/>
+      <c r="K292" s="6"/>
+      <c r="L292" s="6"/>
+      <c r="M292" s="6"/>
+      <c r="N292" s="6"/>
+      <c r="O292" s="6"/>
+      <c r="P292" s="6"/>
+      <c r="Q292" s="6"/>
+      <c r="R292" s="6"/>
+      <c r="S292" s="6"/>
+      <c r="T292" s="6"/>
+    </row>
+    <row r="294" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A294" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C246" s="3">
+      <c r="C294" s="3">
         <v>40335</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="6" t="s">
+    <row r="295" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B247" s="6"/>
-      <c r="C247" s="6"/>
-      <c r="D247" s="6"/>
-      <c r="E247" s="6"/>
-      <c r="F247" s="6"/>
-      <c r="G247" s="6"/>
-      <c r="H247" s="6"/>
-      <c r="I247" s="6"/>
-      <c r="J247" s="6"/>
-      <c r="K247" s="6"/>
-      <c r="L247" s="6"/>
-      <c r="M247" s="6"/>
-      <c r="N247" s="6"/>
-      <c r="O247" s="6"/>
-      <c r="P247" s="6"/>
-      <c r="Q247" s="6"/>
-      <c r="R247" s="6"/>
-      <c r="S247" s="6"/>
-      <c r="T247" s="6"/>
-    </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
+      <c r="B295" s="6"/>
+      <c r="C295" s="6"/>
+      <c r="D295" s="6"/>
+      <c r="E295" s="6"/>
+      <c r="F295" s="6"/>
+      <c r="G295" s="6"/>
+      <c r="H295" s="6"/>
+      <c r="I295" s="6"/>
+      <c r="J295" s="6"/>
+      <c r="K295" s="6"/>
+      <c r="L295" s="6"/>
+      <c r="M295" s="6"/>
+      <c r="N295" s="6"/>
+      <c r="O295" s="6"/>
+      <c r="P295" s="6"/>
+      <c r="Q295" s="6"/>
+      <c r="R295" s="6"/>
+      <c r="S295" s="6"/>
+      <c r="T295" s="6"/>
+    </row>
+    <row r="298" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A298" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C250" s="3">
+      <c r="C298" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
+    <row r="299" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A241:T241"/>
-    <mergeCell ref="A244:T244"/>
-    <mergeCell ref="A247:T247"/>
+    <mergeCell ref="A289:T289"/>
+    <mergeCell ref="A292:T292"/>
+    <mergeCell ref="A295:T295"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B147" r:id="rId1"/>
+    <hyperlink ref="B195" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2490,12 +2924,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2503,12 +2937,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release properly cleaned version this time
</commit_message>
<xml_diff>
--- a/OpenSolver ChangeLog.xlsx
+++ b/OpenSolver ChangeLog.xlsx
@@ -25,7 +25,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$191</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$U$194</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -34,7 +34,7 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="265">
   <si>
     <t>OpenSolver Release Notes</t>
   </si>
@@ -855,6 +855,12 @@
   </si>
   <si>
     <t>Fix error on "Set QuickSolve Parameters" cancel press</t>
+  </si>
+  <si>
+    <t>Version 2.8.2</t>
+  </si>
+  <si>
+    <t>Another fix for "Automation Error"</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1241,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T303"/>
+  <dimension ref="A1:T306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,325 +1262,322 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C3" s="1">
-        <v>42411</v>
+        <v>42414</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C7" s="1">
-        <v>42401</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H8" s="5"/>
+        <v>262</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="H9" s="5"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H10" s="5"/>
+      <c r="A10" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42401</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>215</v>
+      <c r="A12" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>226</v>
+      <c r="A14" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>227</v>
+      <c r="A15" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>217</v>
+      <c r="A17" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>230</v>
+      <c r="A20" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>234</v>
+      <c r="A25" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>220</v>
+      <c r="A27" s="6" t="s">
+        <v>233</v>
       </c>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>221</v>
+      <c r="A29" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>237</v>
+      <c r="A30" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>239</v>
+      <c r="A32" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>222</v>
+      <c r="A50" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C55" s="1">
-        <v>42183</v>
-      </c>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="H56" s="5"/>
     </row>
@@ -1584,232 +1587,235 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C58" s="1">
-        <v>42171</v>
+        <v>42183</v>
       </c>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>204</v>
-      </c>
+      <c r="A60" s="4"/>
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>205</v>
+      <c r="A61" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C61" s="1">
+        <v>42171</v>
       </c>
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C70" s="1">
         <v>42051</v>
-      </c>
-      <c r="H67" s="5"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>186</v>
-      </c>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>187</v>
-      </c>
-      <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>188</v>
       </c>
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>198</v>
+      </c>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>199</v>
+      </c>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>200</v>
+      </c>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>201</v>
       </c>
-      <c r="H83" s="5"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="H84" s="5"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C88" s="1">
         <v>41920</v>
-      </c>
-      <c r="H85" s="5"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="H86" s="5"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H87" s="5"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H91" s="5"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H92" s="5"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
+      <c r="A93" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>176</v>
+      <c r="A94" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H95" s="5"/>
     </row>
@@ -1819,13 +1825,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H98" s="5"/>
     </row>
@@ -1835,1063 +1841,1047 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H100" s="5"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="H101" s="5"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H102" s="5"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-      <c r="H103" s="5"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="H104" s="5"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H105" s="5"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>170</v>
-      </c>
+      <c r="A106" s="2"/>
       <c r="H106" s="5"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>168</v>
+      <c r="A107" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="H107" s="5"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H108" s="5"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
+      <c r="A109" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="H109" s="5"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C110" s="1">
-        <v>41810</v>
+      <c r="A110" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="H110" s="5"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C111" s="1"/>
+        <v>169</v>
+      </c>
       <c r="H111" s="5"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>160</v>
-      </c>
+      <c r="A112" s="2"/>
       <c r="H112" s="5"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
-        <v>164</v>
+      <c r="A113" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C113" s="1">
+        <v>41810</v>
       </c>
       <c r="H113" s="5"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>165</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C114" s="1"/>
       <c r="H114" s="5"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H115" s="5"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H116" s="5"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="2"/>
+      <c r="A117" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="H117" s="5"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C118" s="1">
-        <v>41324</v>
+      <c r="A118" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="H118" s="5"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C119" s="1"/>
+        <v>162</v>
+      </c>
       <c r="H119" s="5"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C120" s="1"/>
+      <c r="A120" s="2"/>
       <c r="H120" s="5"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C121" s="1"/>
+      <c r="A121" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C121" s="1">
+        <v>41324</v>
+      </c>
       <c r="H121" s="5"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C122" s="1"/>
       <c r="H122" s="5"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C123" s="1"/>
       <c r="H123" s="5"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C124" s="1"/>
       <c r="H124" s="5"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C125" s="1"/>
       <c r="H125" s="5"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C126" s="1"/>
       <c r="H126" s="5"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C127" s="1"/>
       <c r="H127" s="5"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C128" s="1"/>
       <c r="H128" s="5"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C129" s="1"/>
       <c r="H129" s="5"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C130" s="1"/>
       <c r="H130" s="5"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C131" s="1"/>
       <c r="H131" s="5"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C132" s="1"/>
       <c r="H132" s="5"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C133" s="1"/>
       <c r="H133" s="5"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C134" s="1"/>
       <c r="H134" s="5"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C135" s="1"/>
       <c r="H135" s="5"/>
     </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C136" s="1"/>
+      <c r="H136" s="5"/>
+    </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C137" s="1"/>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C138" s="1"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C137" s="1">
+      <c r="C140" s="1">
         <v>41211</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="4" t="s">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="4"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C144" s="1">
         <v>41176</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="2"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C145" s="1">
-        <v>41157</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C148" s="1">
+        <v>41157</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="2"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C153" s="1">
         <v>40963</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="2"/>
+      <c r="A155" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C156" s="1">
-        <v>40882</v>
+      <c r="A156" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>123</v>
-      </c>
-      <c r="C157" s="1"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>124</v>
-      </c>
-      <c r="C158" s="1"/>
+      <c r="A158" s="2"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>134</v>
-      </c>
-      <c r="C159" s="1"/>
+      <c r="A159" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C159" s="1">
+        <v>40882</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C160" s="1"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="2"/>
+      <c r="A161" t="s">
+        <v>124</v>
+      </c>
+      <c r="C161" s="1"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C162" s="1">
-        <v>40877</v>
-      </c>
+      <c r="A162" t="s">
+        <v>134</v>
+      </c>
+      <c r="C162" s="1"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>125</v>
+      </c>
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="2"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C165" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>119</v>
       </c>
-      <c r="C163" s="1"/>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="4" t="s">
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C164" s="1"/>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="2"/>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="2"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C167" s="1">
+      <c r="C170" s="1">
         <v>40858</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C168" s="1"/>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>115</v>
-      </c>
+      <c r="C171" s="1"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="2"/>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="2"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C175" s="1">
+      <c r="C178" s="1">
         <v>40815</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="4" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="2"/>
+      <c r="A189" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C190" s="1">
-        <v>40764</v>
+      <c r="A190" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>94</v>
-      </c>
+      <c r="A192" s="2"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>96</v>
-      </c>
-      <c r="B193" s="5"/>
+      <c r="A193" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C193" s="1">
+        <v>40764</v>
+      </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="4"/>
+      <c r="A195" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C196" s="1">
-        <v>40755</v>
-      </c>
+      <c r="A196" t="s">
+        <v>96</v>
+      </c>
+      <c r="B196" s="5"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="4"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C199" s="1">
+        <v>40755</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B199" s="5" t="s">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B202" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="4"/>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>70</v>
-      </c>
+      <c r="A204" s="4"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="4"/>
+      <c r="A208" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
-        <v>76</v>
-      </c>
+      <c r="A211" s="4"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="4"/>
+      <c r="A212" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="4"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B215" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="4"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="4"/>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="4"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="4"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="2"/>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C230" s="1">
-        <v>40731</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="2"/>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C233" s="1">
+        <v>40731</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>60</v>
       </c>
-      <c r="C231" s="1"/>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="4" t="s">
+      <c r="C234" s="1"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C232" s="1"/>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="4" t="s">
+      <c r="C235" s="1"/>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C233" s="1"/>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="4" t="s">
+      <c r="C236" s="1"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C234" s="1"/>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C236" s="1">
-        <v>40610</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>58</v>
-      </c>
+      <c r="C237" s="1"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C239" s="1">
-        <v>40606</v>
+        <v>40610</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242" s="1">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B244" t="s">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B245" t="s">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B246" t="s">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B247" t="s">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B250" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B248" t="s">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B249" t="s">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B251" t="s">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B252" t="s">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B255" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B253" t="s">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B255" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B256" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>19</v>
+      <c r="B259" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
-        <v>18</v>
+      <c r="A260" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B262" t="s">
-        <v>29</v>
+      <c r="A262" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>22</v>
+      <c r="B266" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B269" t="s">
-        <v>31</v>
+      <c r="A269" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>25</v>
+      <c r="B270" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B274" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B276" t="s">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B279" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B278" t="s">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B280" t="s">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="2" t="s">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B285" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B283" t="s">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B284" t="s">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B285" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="2" t="s">
+    <row r="291" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C288" s="3">
+      <c r="C291" s="3">
         <v>40407</v>
       </c>
     </row>
-    <row r="289" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
+    <row r="292" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="292" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A292" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C292" s="3">
-        <v>40375</v>
-      </c>
-    </row>
-    <row r="293" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A293" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B293" s="8"/>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="8"/>
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C295" s="3">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="296" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40375</v>
+      </c>
+    </row>
+    <row r="296" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B296" s="7"/>
-      <c r="C296" s="7"/>
-      <c r="D296" s="7"/>
-      <c r="E296" s="7"/>
-      <c r="F296" s="7"/>
-      <c r="G296" s="7"/>
-      <c r="H296" s="7"/>
-      <c r="I296" s="7"/>
-      <c r="J296" s="7"/>
-      <c r="K296" s="7"/>
-      <c r="L296" s="7"/>
-      <c r="M296" s="7"/>
-      <c r="N296" s="7"/>
-      <c r="O296" s="7"/>
-      <c r="P296" s="7"/>
-      <c r="Q296" s="7"/>
-      <c r="R296" s="7"/>
-      <c r="S296" s="7"/>
-      <c r="T296" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="B296" s="8"/>
+      <c r="C296" s="8"/>
+      <c r="D296" s="8"/>
+      <c r="E296" s="8"/>
+      <c r="F296" s="8"/>
+      <c r="G296" s="8"/>
+      <c r="H296" s="8"/>
+      <c r="I296" s="8"/>
+      <c r="J296" s="8"/>
+      <c r="K296" s="8"/>
+      <c r="L296" s="8"/>
+      <c r="M296" s="8"/>
+      <c r="N296" s="8"/>
+      <c r="O296" s="8"/>
+      <c r="P296" s="8"/>
+      <c r="Q296" s="8"/>
+      <c r="R296" s="8"/>
+      <c r="S296" s="8"/>
+      <c r="T296" s="8"/>
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
@@ -2903,7 +2893,7 @@
     </row>
     <row r="299" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B299" s="7"/>
       <c r="C299" s="7"/>
@@ -2925,27 +2915,59 @@
       <c r="S299" s="7"/>
       <c r="T299" s="7"/>
     </row>
-    <row r="302" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A302" s="2" t="s">
+    <row r="301" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A301" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C301" s="3">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="302" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B302" s="7"/>
+      <c r="C302" s="7"/>
+      <c r="D302" s="7"/>
+      <c r="E302" s="7"/>
+      <c r="F302" s="7"/>
+      <c r="G302" s="7"/>
+      <c r="H302" s="7"/>
+      <c r="I302" s="7"/>
+      <c r="J302" s="7"/>
+      <c r="K302" s="7"/>
+      <c r="L302" s="7"/>
+      <c r="M302" s="7"/>
+      <c r="N302" s="7"/>
+      <c r="O302" s="7"/>
+      <c r="P302" s="7"/>
+      <c r="Q302" s="7"/>
+      <c r="R302" s="7"/>
+      <c r="S302" s="7"/>
+      <c r="T302" s="7"/>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C302" s="3">
+      <c r="C305" s="3">
         <v>40315</v>
       </c>
     </row>
-    <row r="303" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A293:T293"/>
     <mergeCell ref="A296:T296"/>
     <mergeCell ref="A299:T299"/>
+    <mergeCell ref="A302:T302"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B199" r:id="rId1"/>
+    <hyperlink ref="B202" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>